<commit_message>
Foram adicionadas novas bases de dados ao projeto
</commit_message>
<xml_diff>
--- a/calculo_python/pentada_areaDesmatada1.xlsx
+++ b/calculo_python/pentada_areaDesmatada1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,30 +436,80 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2001</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2002</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2003</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2004</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2005</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>2006</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>2007</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>2008</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>2009</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>2010</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2011</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2012</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2013</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2014</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Pentada</t>
         </is>
@@ -467,21 +517,51 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>132580.2662503671</v>
+      </c>
+      <c r="B2" t="n">
+        <v>132518.486381729</v>
+      </c>
+      <c r="C2" t="n">
+        <v>158179.2454899357</v>
+      </c>
+      <c r="D2" t="n">
+        <v>69328.7509945655</v>
+      </c>
+      <c r="E2" t="n">
+        <v>123551.0074646594</v>
+      </c>
+      <c r="F2" t="n">
+        <v>143461.9590245041</v>
+      </c>
+      <c r="G2" t="n">
+        <v>183795.1886348725</v>
+      </c>
+      <c r="H2" t="n">
+        <v>133490.9763442244</v>
+      </c>
+      <c r="I2" t="n">
+        <v>141595.5328419855</v>
+      </c>
+      <c r="J2" t="n">
+        <v>91357.56140417958</v>
+      </c>
+      <c r="K2" t="n">
         <v>96475.37086936354</v>
       </c>
-      <c r="B2" t="n">
+      <c r="L2" t="n">
         <v>110626.3166199554</v>
       </c>
-      <c r="C2" t="n">
+      <c r="M2" t="n">
         <v>145672.8391054713</v>
       </c>
-      <c r="D2" t="n">
+      <c r="N2" t="n">
         <v>131212.7670941408</v>
       </c>
-      <c r="E2" t="n">
+      <c r="O2" t="n">
         <v>80571.10088600834</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>1º</t>
         </is>
@@ -489,21 +569,51 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>187407.4105011359</v>
+      </c>
+      <c r="B3" t="n">
+        <v>147565.7013924507</v>
+      </c>
+      <c r="C3" t="n">
+        <v>188861.6841328789</v>
+      </c>
+      <c r="D3" t="n">
+        <v>94439.96486930861</v>
+      </c>
+      <c r="E3" t="n">
+        <v>202621.795658433</v>
+      </c>
+      <c r="F3" t="n">
+        <v>151254.9071560466</v>
+      </c>
+      <c r="G3" t="n">
+        <v>121426.5467838625</v>
+      </c>
+      <c r="H3" t="n">
+        <v>158411.9753975515</v>
+      </c>
+      <c r="I3" t="n">
+        <v>151863.2346787544</v>
+      </c>
+      <c r="J3" t="n">
+        <v>137491.7995754093</v>
+      </c>
+      <c r="K3" t="n">
         <v>126050.1297278498</v>
       </c>
-      <c r="B3" t="n">
+      <c r="L3" t="n">
         <v>99853.14897546588</v>
       </c>
-      <c r="C3" t="n">
+      <c r="M3" t="n">
         <v>156594.8781708738</v>
       </c>
-      <c r="D3" t="n">
+      <c r="N3" t="n">
         <v>207567.0248510099</v>
       </c>
-      <c r="E3" t="n">
+      <c r="O3" t="n">
         <v>98411.43269858278</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>2º</t>
         </is>
@@ -511,21 +621,51 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
+        <v>134548.2035603131</v>
+      </c>
+      <c r="B4" t="n">
+        <v>150190.4342649275</v>
+      </c>
+      <c r="C4" t="n">
+        <v>143690.1355174568</v>
+      </c>
+      <c r="D4" t="n">
+        <v>115257.9626017626</v>
+      </c>
+      <c r="E4" t="n">
+        <v>192408.5231489593</v>
+      </c>
+      <c r="F4" t="n">
+        <v>170504.4288265377</v>
+      </c>
+      <c r="G4" t="n">
+        <v>203766.597359751</v>
+      </c>
+      <c r="H4" t="n">
+        <v>164369.4545765522</v>
+      </c>
+      <c r="I4" t="n">
+        <v>178216.99017</v>
+      </c>
+      <c r="J4" t="n">
+        <v>88803.9722519333</v>
+      </c>
+      <c r="K4" t="n">
         <v>193649.4596695991</v>
       </c>
-      <c r="B4" t="n">
+      <c r="L4" t="n">
         <v>111040.4832917382</v>
       </c>
-      <c r="C4" t="n">
+      <c r="M4" t="n">
         <v>197065.4177762349</v>
       </c>
-      <c r="D4" t="n">
+      <c r="N4" t="n">
         <v>216416.167393015</v>
       </c>
-      <c r="E4" t="n">
+      <c r="O4" t="n">
         <v>150664.0529895706</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>3º</t>
         </is>
@@ -533,21 +673,51 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
+        <v>118962.7550758586</v>
+      </c>
+      <c r="B5" t="n">
+        <v>187143.5867685429</v>
+      </c>
+      <c r="C5" t="n">
+        <v>167677.4503935514</v>
+      </c>
+      <c r="D5" t="n">
+        <v>182979.0130906197</v>
+      </c>
+      <c r="E5" t="n">
+        <v>184931.9159631691</v>
+      </c>
+      <c r="F5" t="n">
+        <v>81315.2587083705</v>
+      </c>
+      <c r="G5" t="n">
+        <v>142078.1315379197</v>
+      </c>
+      <c r="H5" t="n">
+        <v>67639.19789768477</v>
+      </c>
+      <c r="I5" t="n">
+        <v>107291.4204863173</v>
+      </c>
+      <c r="J5" t="n">
+        <v>228573.0054090609</v>
+      </c>
+      <c r="K5" t="n">
         <v>128997.8752832712</v>
       </c>
-      <c r="B5" t="n">
+      <c r="L5" t="n">
         <v>103387.6079731811</v>
       </c>
-      <c r="C5" t="n">
+      <c r="M5" t="n">
         <v>171382.3862962312</v>
       </c>
-      <c r="D5" t="n">
+      <c r="N5" t="n">
         <v>160916.0105540443</v>
       </c>
-      <c r="E5" t="n">
+      <c r="O5" t="n">
         <v>160901.533868191</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>4º</t>
         </is>
@@ -555,21 +725,51 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
+        <v>77886.97664193164</v>
+      </c>
+      <c r="B6" t="n">
+        <v>119501.7248986973</v>
+      </c>
+      <c r="C6" t="n">
+        <v>53364.42657188523</v>
+      </c>
+      <c r="D6" t="n">
+        <v>225913.9506898005</v>
+      </c>
+      <c r="E6" t="n">
+        <v>163062.2668025148</v>
+      </c>
+      <c r="F6" t="n">
+        <v>82499.81512820294</v>
+      </c>
+      <c r="G6" t="n">
+        <v>135385.5554021049</v>
+      </c>
+      <c r="H6" t="n">
+        <v>130420.9828032401</v>
+      </c>
+      <c r="I6" t="n">
+        <v>187806.2552470639</v>
+      </c>
+      <c r="J6" t="n">
+        <v>114028.6548891704</v>
+      </c>
+      <c r="K6" t="n">
         <v>224983.7614886563</v>
       </c>
-      <c r="B6" t="n">
+      <c r="L6" t="n">
         <v>145192.1436396879</v>
       </c>
-      <c r="C6" t="n">
+      <c r="M6" t="n">
         <v>153476.9340051874</v>
       </c>
-      <c r="D6" t="n">
+      <c r="N6" t="n">
         <v>183411.780966396</v>
       </c>
-      <c r="E6" t="n">
+      <c r="O6" t="n">
         <v>122960.197550553</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>5º</t>
         </is>
@@ -577,21 +777,51 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>258108.9688548594</v>
+      </c>
+      <c r="B7" t="n">
+        <v>172094.2958203857</v>
+      </c>
+      <c r="C7" t="n">
+        <v>114584.9459152072</v>
+      </c>
+      <c r="D7" t="n">
+        <v>153778.8388716529</v>
+      </c>
+      <c r="E7" t="n">
+        <v>154955.6895996132</v>
+      </c>
+      <c r="F7" t="n">
+        <v>167854.5119962954</v>
+      </c>
+      <c r="G7" t="n">
+        <v>138092.6008079005</v>
+      </c>
+      <c r="H7" t="n">
+        <v>210322.7892788456</v>
+      </c>
+      <c r="I7" t="n">
+        <v>229234.6968114967</v>
+      </c>
+      <c r="J7" t="n">
+        <v>260422.636629905</v>
+      </c>
+      <c r="K7" t="n">
         <v>195526.4794348399</v>
       </c>
-      <c r="B7" t="n">
+      <c r="L7" t="n">
         <v>214053.1330940396</v>
       </c>
-      <c r="C7" t="n">
+      <c r="M7" t="n">
         <v>244616.9969638976</v>
       </c>
-      <c r="D7" t="n">
+      <c r="N7" t="n">
         <v>200383.0515885298</v>
       </c>
-      <c r="E7" t="n">
+      <c r="O7" t="n">
         <v>193347.644643163</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>6º</t>
         </is>
@@ -599,21 +829,51 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
+        <v>79401.98937717512</v>
+      </c>
+      <c r="B8" t="n">
+        <v>113794.7810001374</v>
+      </c>
+      <c r="C8" t="n">
+        <v>87098.98456915688</v>
+      </c>
+      <c r="D8" t="n">
+        <v>131778.168539425</v>
+      </c>
+      <c r="E8" t="n">
+        <v>103660.4724219939</v>
+      </c>
+      <c r="F8" t="n">
+        <v>85481.2459483352</v>
+      </c>
+      <c r="G8" t="n">
+        <v>151832.5285777747</v>
+      </c>
+      <c r="H8" t="n">
+        <v>143476.5508411222</v>
+      </c>
+      <c r="I8" t="n">
+        <v>204743.563802966</v>
+      </c>
+      <c r="J8" t="n">
+        <v>140203.0694039362</v>
+      </c>
+      <c r="K8" t="n">
         <v>116075.6928120558</v>
       </c>
-      <c r="B8" t="n">
+      <c r="L8" t="n">
         <v>100108.1085115321</v>
       </c>
-      <c r="C8" t="n">
+      <c r="M8" t="n">
         <v>208587.1133291208</v>
       </c>
-      <c r="D8" t="n">
+      <c r="N8" t="n">
         <v>184273.4988749186</v>
       </c>
-      <c r="E8" t="n">
+      <c r="O8" t="n">
         <v>146191.8725055919</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>7º</t>
         </is>
@@ -621,21 +881,51 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
+        <v>83631.85936637959</v>
+      </c>
+      <c r="B9" t="n">
+        <v>61288.15870450707</v>
+      </c>
+      <c r="C9" t="n">
+        <v>178599.3626809063</v>
+      </c>
+      <c r="D9" t="n">
+        <v>165045.1293166215</v>
+      </c>
+      <c r="E9" t="n">
+        <v>167707.1584713581</v>
+      </c>
+      <c r="F9" t="n">
+        <v>151652.153761224</v>
+      </c>
+      <c r="G9" t="n">
+        <v>230582.4429500805</v>
+      </c>
+      <c r="H9" t="n">
+        <v>147912.9973372739</v>
+      </c>
+      <c r="I9" t="n">
+        <v>113278.9457579146</v>
+      </c>
+      <c r="J9" t="n">
+        <v>161550.2455391157</v>
+      </c>
+      <c r="K9" t="n">
         <v>130120.5401569142</v>
       </c>
-      <c r="B9" t="n">
+      <c r="L9" t="n">
         <v>161005.6760625878</v>
       </c>
-      <c r="C9" t="n">
+      <c r="M9" t="n">
         <v>98755.41866291279</v>
       </c>
-      <c r="D9" t="n">
+      <c r="N9" t="n">
         <v>263411.0767925936</v>
       </c>
-      <c r="E9" t="n">
+      <c r="O9" t="n">
         <v>100702.5590607699</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>8º</t>
         </is>
@@ -643,21 +933,51 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
+        <v>124318.7754562154</v>
+      </c>
+      <c r="B10" t="n">
+        <v>130859.4388458775</v>
+      </c>
+      <c r="C10" t="n">
+        <v>130189.8510644876</v>
+      </c>
+      <c r="D10" t="n">
+        <v>142253.4287869771</v>
+      </c>
+      <c r="E10" t="n">
+        <v>146262.3519194509</v>
+      </c>
+      <c r="F10" t="n">
+        <v>170005.7301510681</v>
+      </c>
+      <c r="G10" t="n">
+        <v>216073.482839966</v>
+      </c>
+      <c r="H10" t="n">
+        <v>114525.4838074479</v>
+      </c>
+      <c r="I10" t="n">
+        <v>129370.7827722212</v>
+      </c>
+      <c r="J10" t="n">
+        <v>166488.4793246101</v>
+      </c>
+      <c r="K10" t="n">
         <v>223002.7807952434</v>
       </c>
-      <c r="B10" t="n">
+      <c r="L10" t="n">
         <v>155405.6178329393</v>
       </c>
-      <c r="C10" t="n">
+      <c r="M10" t="n">
         <v>198429.1135539782</v>
       </c>
-      <c r="D10" t="n">
+      <c r="N10" t="n">
         <v>149719.6070637272</v>
       </c>
-      <c r="E10" t="n">
+      <c r="O10" t="n">
         <v>173352.6562946842</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>9º</t>
         </is>
@@ -665,21 +985,51 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
+        <v>134663.0508984659</v>
+      </c>
+      <c r="B11" t="n">
+        <v>178785.8001050538</v>
+      </c>
+      <c r="C11" t="n">
+        <v>113476.9835658355</v>
+      </c>
+      <c r="D11" t="n">
+        <v>127396.0482360092</v>
+      </c>
+      <c r="E11" t="n">
+        <v>197454.0643355275</v>
+      </c>
+      <c r="F11" t="n">
+        <v>193323.7019803364</v>
+      </c>
+      <c r="G11" t="n">
+        <v>127949.6925576006</v>
+      </c>
+      <c r="H11" t="n">
+        <v>186674.4273945378</v>
+      </c>
+      <c r="I11" t="n">
+        <v>195063.8818212918</v>
+      </c>
+      <c r="J11" t="n">
+        <v>222723.1725465288</v>
+      </c>
+      <c r="K11" t="n">
         <v>141118.5403804854</v>
       </c>
-      <c r="B11" t="n">
+      <c r="L11" t="n">
         <v>183657.717430743</v>
       </c>
-      <c r="C11" t="n">
+      <c r="M11" t="n">
         <v>158142.9155399473</v>
       </c>
-      <c r="D11" t="n">
+      <c r="N11" t="n">
         <v>109915.2741394642</v>
       </c>
-      <c r="E11" t="n">
+      <c r="O11" t="n">
         <v>91401.79750642576</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>10º</t>
         </is>
@@ -687,21 +1037,51 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
+        <v>94463.03531948905</v>
+      </c>
+      <c r="B12" t="n">
+        <v>207007.4419767791</v>
+      </c>
+      <c r="C12" t="n">
+        <v>142069.1180269727</v>
+      </c>
+      <c r="D12" t="n">
+        <v>91668.72978721328</v>
+      </c>
+      <c r="E12" t="n">
+        <v>128778.4872581483</v>
+      </c>
+      <c r="F12" t="n">
+        <v>191117.0918894074</v>
+      </c>
+      <c r="G12" t="n">
+        <v>118162.3983929804</v>
+      </c>
+      <c r="H12" t="n">
+        <v>142669.850970474</v>
+      </c>
+      <c r="I12" t="n">
+        <v>130298.7058167402</v>
+      </c>
+      <c r="J12" t="n">
+        <v>261828.8610361586</v>
+      </c>
+      <c r="K12" t="n">
         <v>109087.0603286219</v>
       </c>
-      <c r="B12" t="n">
+      <c r="L12" t="n">
         <v>142214.6897058377</v>
       </c>
-      <c r="C12" t="n">
+      <c r="M12" t="n">
         <v>147533.6361192144</v>
       </c>
-      <c r="D12" t="n">
+      <c r="N12" t="n">
         <v>184716.9962059692</v>
       </c>
-      <c r="E12" t="n">
+      <c r="O12" t="n">
         <v>171892.2551746669</v>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>11º</t>
         </is>
@@ -709,21 +1089,51 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
+        <v>55773.9726162406</v>
+      </c>
+      <c r="B13" t="n">
+        <v>106736.6358161702</v>
+      </c>
+      <c r="C13" t="n">
+        <v>75619.43636356057</v>
+      </c>
+      <c r="D13" t="n">
+        <v>54756.1110309975</v>
+      </c>
+      <c r="E13" t="n">
+        <v>62857.15624682476</v>
+      </c>
+      <c r="F13" t="n">
+        <v>45911.68937285552</v>
+      </c>
+      <c r="G13" t="n">
+        <v>101480.4451057097</v>
+      </c>
+      <c r="H13" t="n">
+        <v>36117.97740887849</v>
+      </c>
+      <c r="I13" t="n">
+        <v>76374.76596036051</v>
+      </c>
+      <c r="J13" t="n">
+        <v>93453.09806031999</v>
+      </c>
+      <c r="K13" t="n">
         <v>87092.71871030466</v>
       </c>
-      <c r="B13" t="n">
+      <c r="L13" t="n">
         <v>117854.1528557385</v>
       </c>
-      <c r="C13" t="n">
+      <c r="M13" t="n">
         <v>103834.9258473004</v>
       </c>
-      <c r="D13" t="n">
+      <c r="N13" t="n">
         <v>58020.69127015135</v>
       </c>
-      <c r="E13" t="n">
+      <c r="O13" t="n">
         <v>44461.9700601914</v>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="P13" t="inlineStr">
         <is>
           <t>12º</t>
         </is>
@@ -731,21 +1141,51 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
+        <v>132929.1410309137</v>
+      </c>
+      <c r="B14" t="n">
+        <v>125266.4511608723</v>
+      </c>
+      <c r="C14" t="n">
+        <v>88248.29472824548</v>
+      </c>
+      <c r="D14" t="n">
+        <v>147386.9887361042</v>
+      </c>
+      <c r="E14" t="n">
+        <v>116313.8237576279</v>
+      </c>
+      <c r="F14" t="n">
+        <v>245040.2259267772</v>
+      </c>
+      <c r="G14" t="n">
+        <v>111494.9362282024</v>
+      </c>
+      <c r="H14" t="n">
+        <v>141781.2724315868</v>
+      </c>
+      <c r="I14" t="n">
+        <v>177367.425490226</v>
+      </c>
+      <c r="J14" t="n">
+        <v>109855.8442181605</v>
+      </c>
+      <c r="K14" t="n">
         <v>136361.8670216579</v>
       </c>
-      <c r="B14" t="n">
+      <c r="L14" t="n">
         <v>90776.34125132466</v>
       </c>
-      <c r="C14" t="n">
+      <c r="M14" t="n">
         <v>97763.84973003542</v>
       </c>
-      <c r="D14" t="n">
+      <c r="N14" t="n">
         <v>94370.23975313971</v>
       </c>
-      <c r="E14" t="n">
+      <c r="O14" t="n">
         <v>121808.0414339029</v>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="P14" t="inlineStr">
         <is>
           <t>13º</t>
         </is>
@@ -753,21 +1193,51 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
+        <v>211866.581765149</v>
+      </c>
+      <c r="B15" t="n">
+        <v>76214.14266195869</v>
+      </c>
+      <c r="C15" t="n">
+        <v>125803.9772362763</v>
+      </c>
+      <c r="D15" t="n">
+        <v>101863.8908372319</v>
+      </c>
+      <c r="E15" t="n">
+        <v>142042.5606090358</v>
+      </c>
+      <c r="F15" t="n">
+        <v>151230.6622287227</v>
+      </c>
+      <c r="G15" t="n">
+        <v>65770.8587980102</v>
+      </c>
+      <c r="H15" t="n">
+        <v>79399.62244677433</v>
+      </c>
+      <c r="I15" t="n">
+        <v>170554.2438038544</v>
+      </c>
+      <c r="J15" t="n">
+        <v>101815.5523547492</v>
+      </c>
+      <c r="K15" t="n">
         <v>124922.0660891889</v>
       </c>
-      <c r="B15" t="n">
+      <c r="L15" t="n">
         <v>154450.2508449928</v>
       </c>
-      <c r="C15" t="n">
+      <c r="M15" t="n">
         <v>132094.6214093152</v>
       </c>
-      <c r="D15" t="n">
+      <c r="N15" t="n">
         <v>75638.83068465818</v>
       </c>
-      <c r="E15" t="n">
+      <c r="O15" t="n">
         <v>109778.4698019252</v>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="P15" t="inlineStr">
         <is>
           <t>14º</t>
         </is>
@@ -775,21 +1245,51 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
+        <v>109823.513495666</v>
+      </c>
+      <c r="B16" t="n">
+        <v>147315.7947288962</v>
+      </c>
+      <c r="C16" t="n">
+        <v>142826.1210989034</v>
+      </c>
+      <c r="D16" t="n">
+        <v>229780.4490829319</v>
+      </c>
+      <c r="E16" t="n">
+        <v>55506.3236795986</v>
+      </c>
+      <c r="F16" t="n">
+        <v>175323.469771127</v>
+      </c>
+      <c r="G16" t="n">
+        <v>107228.5506880478</v>
+      </c>
+      <c r="H16" t="n">
+        <v>201130.2391032275</v>
+      </c>
+      <c r="I16" t="n">
+        <v>166811.0051760508</v>
+      </c>
+      <c r="J16" t="n">
+        <v>167001.5586803213</v>
+      </c>
+      <c r="K16" t="n">
         <v>292240.2583301918</v>
       </c>
-      <c r="B16" t="n">
+      <c r="L16" t="n">
         <v>168742.8528381946</v>
       </c>
-      <c r="C16" t="n">
+      <c r="M16" t="n">
         <v>136744.5511105855</v>
       </c>
-      <c r="D16" t="n">
+      <c r="N16" t="n">
         <v>88054.47062131099</v>
       </c>
-      <c r="E16" t="n">
+      <c r="O16" t="n">
         <v>142800.7475366481</v>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="P16" t="inlineStr">
         <is>
           <t>15º</t>
         </is>
@@ -797,21 +1297,51 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
+        <v>143562.6687099455</v>
+      </c>
+      <c r="B17" t="n">
+        <v>93328.08160724267</v>
+      </c>
+      <c r="C17" t="n">
+        <v>72289.06402047107</v>
+      </c>
+      <c r="D17" t="n">
+        <v>166557.2330203261</v>
+      </c>
+      <c r="E17" t="n">
+        <v>169000.2237154082</v>
+      </c>
+      <c r="F17" t="n">
+        <v>196304.7800725675</v>
+      </c>
+      <c r="G17" t="n">
+        <v>169637.1654410119</v>
+      </c>
+      <c r="H17" t="n">
+        <v>184727.7236169107</v>
+      </c>
+      <c r="I17" t="n">
+        <v>128799.0315600601</v>
+      </c>
+      <c r="J17" t="n">
+        <v>161246.8161866878</v>
+      </c>
+      <c r="K17" t="n">
         <v>77103.06465230463</v>
       </c>
-      <c r="B17" t="n">
+      <c r="L17" t="n">
         <v>111918.0193584218</v>
       </c>
-      <c r="C17" t="n">
+      <c r="M17" t="n">
         <v>77285.91568097693</v>
       </c>
-      <c r="D17" t="n">
+      <c r="N17" t="n">
         <v>189457.3550147411</v>
       </c>
-      <c r="E17" t="n">
+      <c r="O17" t="n">
         <v>85838.93781622341</v>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="P17" t="inlineStr">
         <is>
           <t>16º</t>
         </is>
@@ -819,21 +1349,51 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
+        <v>87179.63997080926</v>
+      </c>
+      <c r="B18" t="n">
+        <v>80370.48668524416</v>
+      </c>
+      <c r="C18" t="n">
+        <v>105492.678270153</v>
+      </c>
+      <c r="D18" t="n">
+        <v>163109.4656441561</v>
+      </c>
+      <c r="E18" t="n">
+        <v>142196.9374109567</v>
+      </c>
+      <c r="F18" t="n">
+        <v>126890.4804668613</v>
+      </c>
+      <c r="G18" t="n">
+        <v>123551.0646553713</v>
+      </c>
+      <c r="H18" t="n">
+        <v>173100.419419113</v>
+      </c>
+      <c r="I18" t="n">
+        <v>118833.8434426252</v>
+      </c>
+      <c r="J18" t="n">
+        <v>137056.3762548112</v>
+      </c>
+      <c r="K18" t="n">
         <v>115309.0293461931</v>
       </c>
-      <c r="B18" t="n">
+      <c r="L18" t="n">
         <v>129111.0801372379</v>
       </c>
-      <c r="C18" t="n">
+      <c r="M18" t="n">
         <v>106294.7588602178</v>
       </c>
-      <c r="D18" t="n">
+      <c r="N18" t="n">
         <v>175637.9575524049</v>
       </c>
-      <c r="E18" t="n">
+      <c r="O18" t="n">
         <v>212941.0077924541</v>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="P18" t="inlineStr">
         <is>
           <t>17º</t>
         </is>
@@ -841,21 +1401,51 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
+        <v>131989.9919952636</v>
+      </c>
+      <c r="B19" t="n">
+        <v>174087.4401481703</v>
+      </c>
+      <c r="C19" t="n">
+        <v>120345.7883571401</v>
+      </c>
+      <c r="D19" t="n">
+        <v>209395.7569110344</v>
+      </c>
+      <c r="E19" t="n">
+        <v>201884.960868065</v>
+      </c>
+      <c r="F19" t="n">
+        <v>131157.46335625</v>
+      </c>
+      <c r="G19" t="n">
+        <v>171183.7367048</v>
+      </c>
+      <c r="H19" t="n">
+        <v>102265.3472788568</v>
+      </c>
+      <c r="I19" t="n">
+        <v>165306.5809928818</v>
+      </c>
+      <c r="J19" t="n">
+        <v>151864.8020348045</v>
+      </c>
+      <c r="K19" t="n">
         <v>176199.5542773527</v>
       </c>
-      <c r="B19" t="n">
+      <c r="L19" t="n">
         <v>235549.3614539951</v>
       </c>
-      <c r="C19" t="n">
+      <c r="M19" t="n">
         <v>161326.1019287259</v>
       </c>
-      <c r="D19" t="n">
+      <c r="N19" t="n">
         <v>299728.5240085227</v>
       </c>
-      <c r="E19" t="n">
+      <c r="O19" t="n">
         <v>212469.6238978367</v>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="P19" t="inlineStr">
         <is>
           <t>18º</t>
         </is>
@@ -863,21 +1453,51 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
+        <v>102293.6413170384</v>
+      </c>
+      <c r="B20" t="n">
+        <v>96557.35895751498</v>
+      </c>
+      <c r="C20" t="n">
+        <v>98359.28042390867</v>
+      </c>
+      <c r="D20" t="n">
+        <v>99007.46489372273</v>
+      </c>
+      <c r="E20" t="n">
+        <v>84601.26115055269</v>
+      </c>
+      <c r="F20" t="n">
+        <v>114157.2889328975</v>
+      </c>
+      <c r="G20" t="n">
+        <v>152716.4347731498</v>
+      </c>
+      <c r="H20" t="n">
+        <v>68108.28393477657</v>
+      </c>
+      <c r="I20" t="n">
+        <v>143809.3812295576</v>
+      </c>
+      <c r="J20" t="n">
+        <v>82502.84856504925</v>
+      </c>
+      <c r="K20" t="n">
         <v>138956.8229814715</v>
       </c>
-      <c r="B20" t="n">
+      <c r="L20" t="n">
         <v>149003.3935047523</v>
       </c>
-      <c r="C20" t="n">
+      <c r="M20" t="n">
         <v>74828.31172554904</v>
       </c>
-      <c r="D20" t="n">
+      <c r="N20" t="n">
         <v>68274.32303566649</v>
       </c>
-      <c r="E20" t="n">
+      <c r="O20" t="n">
         <v>69163.70192415196</v>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="P20" t="inlineStr">
         <is>
           <t>19º</t>
         </is>
@@ -885,21 +1505,51 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
+        <v>46878.68847316524</v>
+      </c>
+      <c r="B21" t="n">
+        <v>56868.05820939118</v>
+      </c>
+      <c r="C21" t="n">
+        <v>101851.907505039</v>
+      </c>
+      <c r="D21" t="n">
+        <v>158039.9981089686</v>
+      </c>
+      <c r="E21" t="n">
+        <v>116212.1332299757</v>
+      </c>
+      <c r="F21" t="n">
+        <v>30671.343217674</v>
+      </c>
+      <c r="G21" t="n">
+        <v>214798.8531511642</v>
+      </c>
+      <c r="H21" t="n">
+        <v>134340.1758308935</v>
+      </c>
+      <c r="I21" t="n">
+        <v>21131.94608047404</v>
+      </c>
+      <c r="J21" t="n">
+        <v>123224.9029472127</v>
+      </c>
+      <c r="K21" t="n">
         <v>14568.16975859988</v>
       </c>
-      <c r="B21" t="n">
+      <c r="L21" t="n">
         <v>139748.6221579195</v>
       </c>
-      <c r="C21" t="n">
+      <c r="M21" t="n">
         <v>54113.15371562733</v>
       </c>
-      <c r="D21" t="n">
+      <c r="N21" t="n">
         <v>107034.670086711</v>
       </c>
-      <c r="E21" t="n">
+      <c r="O21" t="n">
         <v>53737.5622997097</v>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="P21" t="inlineStr">
         <is>
           <t>20º</t>
         </is>
@@ -907,21 +1557,51 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
+        <v>50850.87826061816</v>
+      </c>
+      <c r="B22" t="n">
+        <v>71453.3679256308</v>
+      </c>
+      <c r="C22" t="n">
+        <v>153298.1071208131</v>
+      </c>
+      <c r="D22" t="n">
+        <v>60003.63997244886</v>
+      </c>
+      <c r="E22" t="n">
+        <v>43890.18661256868</v>
+      </c>
+      <c r="F22" t="n">
+        <v>21508.83673950783</v>
+      </c>
+      <c r="G22" t="n">
+        <v>106021.5963205149</v>
+      </c>
+      <c r="H22" t="n">
+        <v>93380.56764572</v>
+      </c>
+      <c r="I22" t="n">
+        <v>119308.8766414979</v>
+      </c>
+      <c r="J22" t="n">
+        <v>148971.1167528563</v>
+      </c>
+      <c r="K22" t="n">
         <v>6988.342030728097</v>
       </c>
-      <c r="B22" t="n">
+      <c r="L22" t="n">
         <v>108669.1945211111</v>
       </c>
-      <c r="C22" t="n">
+      <c r="M22" t="n">
         <v>89509.35881825989</v>
       </c>
-      <c r="D22" t="n">
+      <c r="N22" t="n">
         <v>69045.72606645375</v>
       </c>
-      <c r="E22" t="n">
+      <c r="O22" t="n">
         <v>56431.43300973853</v>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="P22" t="inlineStr">
         <is>
           <t>21º</t>
         </is>
@@ -929,21 +1609,51 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
+        <v>100642.9053497202</v>
+      </c>
+      <c r="B23" t="n">
+        <v>52077.16740426924</v>
+      </c>
+      <c r="C23" t="n">
+        <v>35852.89417791956</v>
+      </c>
+      <c r="D23" t="n">
+        <v>94853.78771544804</v>
+      </c>
+      <c r="E23" t="n">
+        <v>92172.68361660076</v>
+      </c>
+      <c r="F23" t="n">
+        <v>56405.82168473639</v>
+      </c>
+      <c r="G23" t="n">
+        <v>35865.68863420392</v>
+      </c>
+      <c r="H23" t="n">
+        <v>81181.64968654592</v>
+      </c>
+      <c r="I23" t="n">
+        <v>37209.42493908637</v>
+      </c>
+      <c r="J23" t="n">
+        <v>103459.0562355714</v>
+      </c>
+      <c r="K23" t="n">
         <v>24189.11541629727</v>
       </c>
-      <c r="B23" t="n">
+      <c r="L23" t="n">
         <v>36600.87048592266</v>
       </c>
-      <c r="C23" t="n">
+      <c r="M23" t="n">
         <v>100379.986825913</v>
       </c>
-      <c r="D23" t="n">
+      <c r="N23" t="n">
         <v>57938.43670715261</v>
       </c>
-      <c r="E23" t="n">
+      <c r="O23" t="n">
         <v>104397.2321824392</v>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="P23" t="inlineStr">
         <is>
           <t>22º</t>
         </is>
@@ -951,21 +1661,51 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
+        <v>57841.99203800131</v>
+      </c>
+      <c r="B24" t="n">
+        <v>162518.3296927807</v>
+      </c>
+      <c r="C24" t="n">
+        <v>56147.48632994352</v>
+      </c>
+      <c r="D24" t="n">
+        <v>58369.31853641156</v>
+      </c>
+      <c r="E24" t="n">
+        <v>99170.38238596451</v>
+      </c>
+      <c r="F24" t="n">
+        <v>78706.74383072201</v>
+      </c>
+      <c r="G24" t="n">
+        <v>61436.02064950838</v>
+      </c>
+      <c r="H24" t="n">
+        <v>55429.78182595949</v>
+      </c>
+      <c r="I24" t="n">
+        <v>99053.89300725285</v>
+      </c>
+      <c r="J24" t="n">
+        <v>160629.2650011213</v>
+      </c>
+      <c r="K24" t="n">
         <v>38874.60175176877</v>
       </c>
-      <c r="B24" t="n">
+      <c r="L24" t="n">
         <v>41546.41512847509</v>
       </c>
-      <c r="C24" t="n">
+      <c r="M24" t="n">
         <v>66448.20954016893</v>
       </c>
-      <c r="D24" t="n">
+      <c r="N24" t="n">
         <v>8678.350903031642</v>
       </c>
-      <c r="E24" t="n">
+      <c r="O24" t="n">
         <v>190615.4104030649</v>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="P24" t="inlineStr">
         <is>
           <t>23º</t>
         </is>
@@ -973,21 +1713,51 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
+        <v>46590.39161029186</v>
+      </c>
+      <c r="B25" t="n">
+        <v>31064.37312052648</v>
+      </c>
+      <c r="C25" t="n">
+        <v>76582.93729787545</v>
+      </c>
+      <c r="D25" t="n">
+        <v>13725.43521068446</v>
+      </c>
+      <c r="E25" t="n">
+        <v>36716.67139968359</v>
+      </c>
+      <c r="F25" t="n">
+        <v>14461.96447213536</v>
+      </c>
+      <c r="G25" t="n">
+        <v>25115.31931609498</v>
+      </c>
+      <c r="H25" t="n">
+        <v>77006.87654688602</v>
+      </c>
+      <c r="I25" t="n">
+        <v>56914.20276744413</v>
+      </c>
+      <c r="J25" t="n">
+        <v>51972.25273611243</v>
+      </c>
+      <c r="K25" t="n">
         <v>19834.89389706079</v>
       </c>
-      <c r="B25" t="n">
+      <c r="L25" t="n">
         <v>27043.06883102285</v>
       </c>
-      <c r="C25" t="n">
+      <c r="M25" t="n">
         <v>93186.00324101168</v>
       </c>
-      <c r="D25" t="n">
+      <c r="N25" t="n">
         <v>47316.18596171119</v>
       </c>
-      <c r="E25" t="n">
+      <c r="O25" t="n">
         <v>105260.1271341997</v>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="P25" t="inlineStr">
         <is>
           <t>24º</t>
         </is>
@@ -995,21 +1765,51 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
+        <v>22994.01338395324</v>
+      </c>
+      <c r="B26" t="n">
+        <v>32398.71149959745</v>
+      </c>
+      <c r="C26" t="n">
+        <v>32647.02100241863</v>
+      </c>
+      <c r="D26" t="n">
+        <v>79069.1817118789</v>
+      </c>
+      <c r="E26" t="n">
+        <v>61436.84280444312</v>
+      </c>
+      <c r="F26" t="n">
+        <v>24396.39568218953</v>
+      </c>
+      <c r="G26" t="n">
+        <v>17345.94540973693</v>
+      </c>
+      <c r="H26" t="n">
+        <v>58887.19613315915</v>
+      </c>
+      <c r="I26" t="n">
+        <v>11635.15989360013</v>
+      </c>
+      <c r="J26" t="n">
+        <v>18240.02179051638</v>
+      </c>
+      <c r="K26" t="n">
         <v>42034.51196191033</v>
       </c>
-      <c r="B26" t="n">
+      <c r="L26" t="n">
         <v>29979.47882921275</v>
       </c>
-      <c r="C26" t="n">
+      <c r="M26" t="n">
         <v>5065.861181874836</v>
       </c>
-      <c r="D26" t="n">
+      <c r="N26" t="n">
         <v>20962.22251965669</v>
       </c>
-      <c r="E26" t="n">
+      <c r="O26" t="n">
         <v>58088.64898886587</v>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="P26" t="inlineStr">
         <is>
           <t>25º</t>
         </is>
@@ -1017,21 +1817,51 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
+        <v>15918.67345519789</v>
+      </c>
+      <c r="B27" t="n">
+        <v>28320.77398917438</v>
+      </c>
+      <c r="C27" t="n">
+        <v>52588.5800277673</v>
+      </c>
+      <c r="D27" t="n">
+        <v>44887.44419396441</v>
+      </c>
+      <c r="E27" t="n">
+        <v>6614.820499913368</v>
+      </c>
+      <c r="F27" t="n">
+        <v>61458.65801524187</v>
+      </c>
+      <c r="G27" t="n">
+        <v>4517.78377550209</v>
+      </c>
+      <c r="H27" t="n">
+        <v>24063.80606464593</v>
+      </c>
+      <c r="I27" t="n">
+        <v>101647.6503630572</v>
+      </c>
+      <c r="J27" t="n">
+        <v>52886.9496875782</v>
+      </c>
+      <c r="K27" t="n">
         <v>48689.60968677101</v>
       </c>
-      <c r="B27" t="n">
+      <c r="L27" t="n">
         <v>18687.5424498233</v>
       </c>
-      <c r="C27" t="n">
+      <c r="M27" t="n">
         <v>6094.375368736998</v>
       </c>
-      <c r="D27" t="n">
+      <c r="N27" t="n">
         <v>29247.07914522207</v>
       </c>
-      <c r="E27" t="n">
+      <c r="O27" t="n">
         <v>64282.84829353446</v>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="P27" t="inlineStr">
         <is>
           <t>26º</t>
         </is>
@@ -1039,21 +1869,51 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
+        <v>30153.86798622374</v>
+      </c>
+      <c r="B28" t="n">
+        <v>75786.19153998133</v>
+      </c>
+      <c r="C28" t="n">
+        <v>42408.22988449448</v>
+      </c>
+      <c r="D28" t="n">
+        <v>23103.1372512663</v>
+      </c>
+      <c r="E28" t="n">
+        <v>21808.50432093145</v>
+      </c>
+      <c r="F28" t="n">
+        <v>9093.434436601992</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3981.998455253071</v>
+      </c>
+      <c r="H28" t="n">
+        <v>4282.890480087548</v>
+      </c>
+      <c r="I28" t="n">
+        <v>65204.05663804642</v>
+      </c>
+      <c r="J28" t="n">
+        <v>86805.79429040042</v>
+      </c>
+      <c r="K28" t="n">
         <v>4719.209497463239</v>
       </c>
-      <c r="B28" t="n">
+      <c r="L28" t="n">
         <v>8720.689440527158</v>
       </c>
-      <c r="C28" t="n">
+      <c r="M28" t="n">
         <v>46141.22864334438</v>
       </c>
-      <c r="D28" t="n">
+      <c r="N28" t="n">
         <v>59698.09384835934</v>
       </c>
-      <c r="E28" t="n">
+      <c r="O28" t="n">
         <v>53153.84267374487</v>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="P28" t="inlineStr">
         <is>
           <t>27º</t>
         </is>
@@ -1061,21 +1921,51 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
+        <v>13774.20239711287</v>
+      </c>
+      <c r="B29" t="n">
+        <v>7282.005816394441</v>
+      </c>
+      <c r="C29" t="n">
+        <v>13787.63042534192</v>
+      </c>
+      <c r="D29" t="n">
+        <v>6389.474320128861</v>
+      </c>
+      <c r="E29" t="n">
+        <v>6353.394155219261</v>
+      </c>
+      <c r="F29" t="n">
+        <v>6264.662466555014</v>
+      </c>
+      <c r="G29" t="n">
+        <v>45624.72071725759</v>
+      </c>
+      <c r="H29" t="n">
+        <v>57076.77608256054</v>
+      </c>
+      <c r="I29" t="n">
+        <v>28311.34161806714</v>
+      </c>
+      <c r="J29" t="n">
+        <v>60288.02119193171</v>
+      </c>
+      <c r="K29" t="n">
         <v>16368.03100606227</v>
       </c>
-      <c r="B29" t="n">
+      <c r="L29" t="n">
         <v>10502.26493617997</v>
       </c>
-      <c r="C29" t="n">
+      <c r="M29" t="n">
         <v>70664.84774950628</v>
       </c>
-      <c r="D29" t="n">
+      <c r="N29" t="n">
         <v>10313.18952618534</v>
       </c>
-      <c r="E29" t="n">
+      <c r="O29" t="n">
         <v>102433.5130325691</v>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="P29" t="inlineStr">
         <is>
           <t>28º</t>
         </is>
@@ -1083,21 +1973,51 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
+        <v>7051.19609577398</v>
+      </c>
+      <c r="B30" t="n">
+        <v>40491.53161274961</v>
+      </c>
+      <c r="C30" t="n">
+        <v>33831.3654260098</v>
+      </c>
+      <c r="D30" t="n">
+        <v>59124.43862673626</v>
+      </c>
+      <c r="E30" t="n">
+        <v>44728.90105279289</v>
+      </c>
+      <c r="F30" t="n">
+        <v>24910.90745147162</v>
+      </c>
+      <c r="G30" t="n">
+        <v>65762.7072248702</v>
+      </c>
+      <c r="H30" t="n">
+        <v>51128.09404783619</v>
+      </c>
+      <c r="I30" t="n">
+        <v>6520.404190178943</v>
+      </c>
+      <c r="J30" t="n">
+        <v>48846.30770703431</v>
+      </c>
+      <c r="K30" t="n">
         <v>28790.4916897241</v>
       </c>
-      <c r="B30" t="n">
+      <c r="L30" t="n">
         <v>22911.96355591097</v>
       </c>
-      <c r="C30" t="n">
+      <c r="M30" t="n">
         <v>88751.05409204448</v>
       </c>
-      <c r="D30" t="n">
+      <c r="N30" t="n">
         <v>20541.76815733092</v>
       </c>
-      <c r="E30" t="n">
+      <c r="O30" t="n">
         <v>49278.97558928052</v>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="P30" t="inlineStr">
         <is>
           <t>29º</t>
         </is>
@@ -1105,21 +2025,51 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
+        <v>6588.127290551338</v>
+      </c>
+      <c r="B31" t="n">
+        <v>63698.64857048328</v>
+      </c>
+      <c r="C31" t="n">
+        <v>18523.88856893472</v>
+      </c>
+      <c r="D31" t="n">
+        <v>91018.64437507083</v>
+      </c>
+      <c r="E31" t="n">
+        <v>11832.20187610201</v>
+      </c>
+      <c r="F31" t="n">
+        <v>77275.95971983371</v>
+      </c>
+      <c r="G31" t="n">
+        <v>17952.08630983642</v>
+      </c>
+      <c r="H31" t="n">
+        <v>6325.645188822001</v>
+      </c>
+      <c r="I31" t="n">
+        <v>67251.22882154364</v>
+      </c>
+      <c r="J31" t="n">
+        <v>57590.3431697991</v>
+      </c>
+      <c r="K31" t="n">
         <v>115112.7113021364</v>
       </c>
-      <c r="B31" t="n">
+      <c r="L31" t="n">
         <v>7054.348128260358</v>
       </c>
-      <c r="C31" t="n">
+      <c r="M31" t="n">
         <v>12702.23543915608</v>
       </c>
-      <c r="D31" t="n">
+      <c r="N31" t="n">
         <v>39057.29165959825</v>
       </c>
-      <c r="E31" t="n">
+      <c r="O31" t="n">
         <v>7110.386174411631</v>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="P31" t="inlineStr">
         <is>
           <t>30º</t>
         </is>
@@ -1127,21 +2077,51 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
+        <v>7057.605935283393</v>
+      </c>
+      <c r="B32" t="n">
+        <v>60891.398675251</v>
+      </c>
+      <c r="C32" t="n">
+        <v>5046.665636652596</v>
+      </c>
+      <c r="D32" t="n">
+        <v>40030.71239867486</v>
+      </c>
+      <c r="E32" t="n">
+        <v>8057.032896475471</v>
+      </c>
+      <c r="F32" t="n">
+        <v>4070.753273266204</v>
+      </c>
+      <c r="G32" t="n">
+        <v>7885.254622182188</v>
+      </c>
+      <c r="H32" t="n">
+        <v>3261.199548820418</v>
+      </c>
+      <c r="I32" t="n">
+        <v>4397.099636957696</v>
+      </c>
+      <c r="J32" t="n">
+        <v>4599.531947255606</v>
+      </c>
+      <c r="K32" t="n">
         <v>30411.22605883609</v>
       </c>
-      <c r="B32" t="n">
+      <c r="L32" t="n">
         <v>3367.240869471842</v>
       </c>
-      <c r="C32" t="n">
+      <c r="M32" t="n">
         <v>29361.20753999249</v>
       </c>
-      <c r="D32" t="n">
+      <c r="N32" t="n">
         <v>28625.94489874934</v>
       </c>
-      <c r="E32" t="n">
+      <c r="O32" t="n">
         <v>4526.771871719407</v>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="P32" t="inlineStr">
         <is>
           <t>31º</t>
         </is>
@@ -1149,21 +2129,51 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
+        <v>3777.474987720391</v>
+      </c>
+      <c r="B33" t="n">
+        <v>15808.22465412476</v>
+      </c>
+      <c r="C33" t="n">
+        <v>4830.716397485316</v>
+      </c>
+      <c r="D33" t="n">
+        <v>5813.810770528922</v>
+      </c>
+      <c r="E33" t="n">
+        <v>28050.45922549684</v>
+      </c>
+      <c r="F33" t="n">
+        <v>4081.440435289633</v>
+      </c>
+      <c r="G33" t="n">
+        <v>3482.5036811097</v>
+      </c>
+      <c r="H33" t="n">
+        <v>3619.5689757665</v>
+      </c>
+      <c r="I33" t="n">
+        <v>2809.152833911486</v>
+      </c>
+      <c r="J33" t="n">
+        <v>7890.797230875251</v>
+      </c>
+      <c r="K33" t="n">
         <v>3408.880029326558</v>
       </c>
-      <c r="B33" t="n">
+      <c r="L33" t="n">
         <v>6494.641549278241</v>
       </c>
-      <c r="C33" t="n">
+      <c r="M33" t="n">
         <v>20171.75012586071</v>
       </c>
-      <c r="D33" t="n">
+      <c r="N33" t="n">
         <v>53822.09074107339</v>
       </c>
-      <c r="E33" t="n">
+      <c r="O33" t="n">
         <v>28331.08015411906</v>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="P33" t="inlineStr">
         <is>
           <t>32º</t>
         </is>
@@ -1171,21 +2181,51 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
+        <v>8273.153064148568</v>
+      </c>
+      <c r="B34" t="n">
+        <v>6634.464004495566</v>
+      </c>
+      <c r="C34" t="n">
+        <v>4449.565251804332</v>
+      </c>
+      <c r="D34" t="n">
+        <v>4499.733388510873</v>
+      </c>
+      <c r="E34" t="n">
+        <v>5438.270665046162</v>
+      </c>
+      <c r="F34" t="n">
+        <v>4486.006806528328</v>
+      </c>
+      <c r="G34" t="n">
+        <v>10450.85744436931</v>
+      </c>
+      <c r="H34" t="n">
+        <v>3989.115440448943</v>
+      </c>
+      <c r="I34" t="n">
+        <v>9313.526669956651</v>
+      </c>
+      <c r="J34" t="n">
+        <v>21339.110553335</v>
+      </c>
+      <c r="K34" t="n">
         <v>3516.947127421114</v>
       </c>
-      <c r="B34" t="n">
+      <c r="L34" t="n">
         <v>8955.360780746803</v>
       </c>
-      <c r="C34" t="n">
+      <c r="M34" t="n">
         <v>5658.178005574729</v>
       </c>
-      <c r="D34" t="n">
+      <c r="N34" t="n">
         <v>5849.074566906805</v>
       </c>
-      <c r="E34" t="n">
+      <c r="O34" t="n">
         <v>16528.10904448758</v>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="P34" t="inlineStr">
         <is>
           <t>33º</t>
         </is>
@@ -1193,21 +2233,51 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
+        <v>9272.25989797209</v>
+      </c>
+      <c r="B35" t="n">
+        <v>35788.41468872467</v>
+      </c>
+      <c r="C35" t="n">
+        <v>3797.724932575461</v>
+      </c>
+      <c r="D35" t="n">
+        <v>3726.250222791411</v>
+      </c>
+      <c r="E35" t="n">
+        <v>9772.41827532917</v>
+      </c>
+      <c r="F35" t="n">
+        <v>7639.526306676868</v>
+      </c>
+      <c r="G35" t="n">
+        <v>3775.372061807741</v>
+      </c>
+      <c r="H35" t="n">
+        <v>3766.284424710977</v>
+      </c>
+      <c r="I35" t="n">
+        <v>3091.846325011112</v>
+      </c>
+      <c r="J35" t="n">
+        <v>21635.36914764694</v>
+      </c>
+      <c r="K35" t="n">
         <v>3795.670939884347</v>
       </c>
-      <c r="B35" t="n">
+      <c r="L35" t="n">
         <v>3536.483279536286</v>
       </c>
-      <c r="C35" t="n">
+      <c r="M35" t="n">
         <v>5507.64589115942</v>
       </c>
-      <c r="D35" t="n">
+      <c r="N35" t="n">
         <v>35421.8236674374</v>
       </c>
-      <c r="E35" t="n">
+      <c r="O35" t="n">
         <v>5307.541689210309</v>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="P35" t="inlineStr">
         <is>
           <t>34º</t>
         </is>
@@ -1215,21 +2285,51 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
+        <v>3976.301107144589</v>
+      </c>
+      <c r="B36" t="n">
+        <v>4100.188753918809</v>
+      </c>
+      <c r="C36" t="n">
+        <v>3471.566325374913</v>
+      </c>
+      <c r="D36" t="n">
+        <v>13581.75927386705</v>
+      </c>
+      <c r="E36" t="n">
+        <v>5934.177477083489</v>
+      </c>
+      <c r="F36" t="n">
+        <v>7287.62875723606</v>
+      </c>
+      <c r="G36" t="n">
+        <v>3500.256752249074</v>
+      </c>
+      <c r="H36" t="n">
+        <v>3150.618248564589</v>
+      </c>
+      <c r="I36" t="n">
+        <v>6101.488596570733</v>
+      </c>
+      <c r="J36" t="n">
+        <v>12513.60542534378</v>
+      </c>
+      <c r="K36" t="n">
         <v>3701.027120775103</v>
       </c>
-      <c r="B36" t="n">
+      <c r="L36" t="n">
         <v>3621.612267840608</v>
       </c>
-      <c r="C36" t="n">
+      <c r="M36" t="n">
         <v>21329.02473355764</v>
       </c>
-      <c r="D36" t="n">
+      <c r="N36" t="n">
         <v>30194.6151245115</v>
       </c>
-      <c r="E36" t="n">
+      <c r="O36" t="n">
         <v>5408.219291772329</v>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="P36" t="inlineStr">
         <is>
           <t>35º</t>
         </is>
@@ -1237,21 +2337,51 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
+        <v>5376.503448815433</v>
+      </c>
+      <c r="B37" t="n">
+        <v>3754.847772712801</v>
+      </c>
+      <c r="C37" t="n">
+        <v>3374.502278465619</v>
+      </c>
+      <c r="D37" t="n">
+        <v>10305.58336320787</v>
+      </c>
+      <c r="E37" t="n">
+        <v>4349.287392139669</v>
+      </c>
+      <c r="F37" t="n">
+        <v>9692.975418627027</v>
+      </c>
+      <c r="G37" t="n">
+        <v>3548.529832161877</v>
+      </c>
+      <c r="H37" t="n">
+        <v>2954.859753530868</v>
+      </c>
+      <c r="I37" t="n">
+        <v>2895.111417835368</v>
+      </c>
+      <c r="J37" t="n">
+        <v>6107.955366038575</v>
+      </c>
+      <c r="K37" t="n">
         <v>3430.345802150757</v>
       </c>
-      <c r="B37" t="n">
+      <c r="L37" t="n">
         <v>4514.194717223742</v>
       </c>
-      <c r="C37" t="n">
+      <c r="M37" t="n">
         <v>9406.335678816786</v>
       </c>
-      <c r="D37" t="n">
+      <c r="N37" t="n">
         <v>40056.07291940029</v>
       </c>
-      <c r="E37" t="n">
+      <c r="O37" t="n">
         <v>4326.330602004945</v>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="P37" t="inlineStr">
         <is>
           <t>36º</t>
         </is>
@@ -1259,21 +2389,51 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
+        <v>13437.10583477349</v>
+      </c>
+      <c r="B38" t="n">
+        <v>8595.468054399294</v>
+      </c>
+      <c r="C38" t="n">
+        <v>7376.196273663697</v>
+      </c>
+      <c r="D38" t="n">
+        <v>3223.600523296291</v>
+      </c>
+      <c r="E38" t="n">
+        <v>12311.96897206283</v>
+      </c>
+      <c r="F38" t="n">
+        <v>3871.001434144558</v>
+      </c>
+      <c r="G38" t="n">
+        <v>3642.921630143186</v>
+      </c>
+      <c r="H38" t="n">
+        <v>3661.63202286573</v>
+      </c>
+      <c r="I38" t="n">
+        <v>3342.088625027271</v>
+      </c>
+      <c r="J38" t="n">
+        <v>6175.506781963393</v>
+      </c>
+      <c r="K38" t="n">
         <v>4700.728099096521</v>
       </c>
-      <c r="B38" t="n">
+      <c r="L38" t="n">
         <v>3733.477878550691</v>
       </c>
-      <c r="C38" t="n">
+      <c r="M38" t="n">
         <v>3383.937675516749</v>
       </c>
-      <c r="D38" t="n">
+      <c r="N38" t="n">
         <v>20270.40948920203</v>
       </c>
-      <c r="E38" t="n">
+      <c r="O38" t="n">
         <v>4675.082020889775</v>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="P38" t="inlineStr">
         <is>
           <t>37º</t>
         </is>
@@ -1281,21 +2441,51 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
+        <v>12898.06605123351</v>
+      </c>
+      <c r="B39" t="n">
+        <v>12967.77864293467</v>
+      </c>
+      <c r="C39" t="n">
+        <v>3446.55873378153</v>
+      </c>
+      <c r="D39" t="n">
+        <v>6153.724336296906</v>
+      </c>
+      <c r="E39" t="n">
+        <v>5833.420133194967</v>
+      </c>
+      <c r="F39" t="n">
+        <v>2660.906432171428</v>
+      </c>
+      <c r="G39" t="n">
+        <v>3084.646008732856</v>
+      </c>
+      <c r="H39" t="n">
+        <v>3195.707230152221</v>
+      </c>
+      <c r="I39" t="n">
+        <v>2907.607681939061</v>
+      </c>
+      <c r="J39" t="n">
+        <v>3918.741106879479</v>
+      </c>
+      <c r="K39" t="n">
         <v>4325.703944223187</v>
       </c>
-      <c r="B39" t="n">
+      <c r="L39" t="n">
         <v>2770.122722053055</v>
       </c>
-      <c r="C39" t="n">
+      <c r="M39" t="n">
         <v>3017.67097385549</v>
       </c>
-      <c r="D39" t="n">
+      <c r="N39" t="n">
         <v>4809.532463862149</v>
       </c>
-      <c r="E39" t="n">
+      <c r="O39" t="n">
         <v>4775.020713925126</v>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="P39" t="inlineStr">
         <is>
           <t>38º</t>
         </is>
@@ -1303,21 +2493,51 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
+        <v>11976.52105399195</v>
+      </c>
+      <c r="B40" t="n">
+        <v>3661.745785535437</v>
+      </c>
+      <c r="C40" t="n">
+        <v>3259.66106622523</v>
+      </c>
+      <c r="D40" t="n">
+        <v>2872.157055265994</v>
+      </c>
+      <c r="E40" t="n">
+        <v>11414.58548933081</v>
+      </c>
+      <c r="F40" t="n">
+        <v>2309.900407282395</v>
+      </c>
+      <c r="G40" t="n">
+        <v>2875.810888494698</v>
+      </c>
+      <c r="H40" t="n">
+        <v>3651.389456550981</v>
+      </c>
+      <c r="I40" t="n">
+        <v>2728.856403404239</v>
+      </c>
+      <c r="J40" t="n">
+        <v>3020.981387471333</v>
+      </c>
+      <c r="K40" t="n">
         <v>9718.242899235207</v>
       </c>
-      <c r="B40" t="n">
+      <c r="L40" t="n">
         <v>3457.802817139091</v>
       </c>
-      <c r="C40" t="n">
+      <c r="M40" t="n">
         <v>2722.730407699064</v>
       </c>
-      <c r="D40" t="n">
+      <c r="N40" t="n">
         <v>3634.817377013087</v>
       </c>
-      <c r="E40" t="n">
+      <c r="O40" t="n">
         <v>3083.071798951367</v>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="P40" t="inlineStr">
         <is>
           <t>39º</t>
         </is>
@@ -1325,21 +2545,51 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
+        <v>3601.072957774588</v>
+      </c>
+      <c r="B41" t="n">
+        <v>3451.282748338053</v>
+      </c>
+      <c r="C41" t="n">
+        <v>27926.77102975006</v>
+      </c>
+      <c r="D41" t="n">
+        <v>2530.062411229397</v>
+      </c>
+      <c r="E41" t="n">
+        <v>5344.809486564002</v>
+      </c>
+      <c r="F41" t="n">
+        <v>2575.841366197199</v>
+      </c>
+      <c r="G41" t="n">
+        <v>2802.636817001709</v>
+      </c>
+      <c r="H41" t="n">
+        <v>16335.92184972458</v>
+      </c>
+      <c r="I41" t="n">
+        <v>2662.732128538689</v>
+      </c>
+      <c r="J41" t="n">
+        <v>3326.63952482705</v>
+      </c>
+      <c r="K41" t="n">
         <v>3574.444396028915</v>
       </c>
-      <c r="B41" t="n">
+      <c r="L41" t="n">
         <v>2815.749270746873</v>
       </c>
-      <c r="C41" t="n">
+      <c r="M41" t="n">
         <v>2812.958919940278</v>
       </c>
-      <c r="D41" t="n">
+      <c r="N41" t="n">
         <v>4895.152687416245</v>
       </c>
-      <c r="E41" t="n">
+      <c r="O41" t="n">
         <v>7630.536512938204</v>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="P41" t="inlineStr">
         <is>
           <t>40º</t>
         </is>
@@ -1347,21 +2597,51 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
+        <v>12202.35913779618</v>
+      </c>
+      <c r="B42" t="n">
+        <v>25449.54009704803</v>
+      </c>
+      <c r="C42" t="n">
+        <v>5743.303496816122</v>
+      </c>
+      <c r="D42" t="n">
+        <v>3264.430819587615</v>
+      </c>
+      <c r="E42" t="n">
+        <v>4886.004952233675</v>
+      </c>
+      <c r="F42" t="n">
+        <v>2853.46887453923</v>
+      </c>
+      <c r="G42" t="n">
+        <v>3723.394427926401</v>
+      </c>
+      <c r="H42" t="n">
+        <v>21150.60942740725</v>
+      </c>
+      <c r="I42" t="n">
+        <v>4112.89168560622</v>
+      </c>
+      <c r="J42" t="n">
+        <v>16749.6374494118</v>
+      </c>
+      <c r="K42" t="n">
         <v>4498.392101139649</v>
       </c>
-      <c r="B42" t="n">
+      <c r="L42" t="n">
         <v>3769.484624509954</v>
       </c>
-      <c r="C42" t="n">
+      <c r="M42" t="n">
         <v>4868.442734408151</v>
       </c>
-      <c r="D42" t="n">
+      <c r="N42" t="n">
         <v>16860.6641721901</v>
       </c>
-      <c r="E42" t="n">
+      <c r="O42" t="n">
         <v>7786.743071235866</v>
       </c>
-      <c r="F42" t="inlineStr">
+      <c r="P42" t="inlineStr">
         <is>
           <t>41º</t>
         </is>
@@ -1369,21 +2649,51 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
+        <v>14867.58946116789</v>
+      </c>
+      <c r="B43" t="n">
+        <v>22101.77600660346</v>
+      </c>
+      <c r="C43" t="n">
+        <v>40287.45398558029</v>
+      </c>
+      <c r="D43" t="n">
+        <v>5505.188248477494</v>
+      </c>
+      <c r="E43" t="n">
+        <v>8433.882491491358</v>
+      </c>
+      <c r="F43" t="n">
+        <v>5292.412483490682</v>
+      </c>
+      <c r="G43" t="n">
+        <v>13061.87388845331</v>
+      </c>
+      <c r="H43" t="n">
+        <v>37127.89021996983</v>
+      </c>
+      <c r="I43" t="n">
+        <v>5797.691174352871</v>
+      </c>
+      <c r="J43" t="n">
+        <v>11015.18543235951</v>
+      </c>
+      <c r="K43" t="n">
         <v>7513.009079620887</v>
       </c>
-      <c r="B43" t="n">
+      <c r="L43" t="n">
         <v>5901.255047717749</v>
       </c>
-      <c r="C43" t="n">
+      <c r="M43" t="n">
         <v>7281.813663829527</v>
       </c>
-      <c r="D43" t="n">
+      <c r="N43" t="n">
         <v>8721.12850061632</v>
       </c>
-      <c r="E43" t="n">
+      <c r="O43" t="n">
         <v>8776.850312698114</v>
       </c>
-      <c r="F43" t="inlineStr">
+      <c r="P43" t="inlineStr">
         <is>
           <t>42º</t>
         </is>
@@ -1391,21 +2701,51 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
+        <v>18538.02688393456</v>
+      </c>
+      <c r="B44" t="n">
+        <v>6357.670092838181</v>
+      </c>
+      <c r="C44" t="n">
+        <v>48837.46936175084</v>
+      </c>
+      <c r="D44" t="n">
+        <v>6806.516794899168</v>
+      </c>
+      <c r="E44" t="n">
+        <v>8449.919885494792</v>
+      </c>
+      <c r="F44" t="n">
+        <v>6055.42166543778</v>
+      </c>
+      <c r="G44" t="n">
+        <v>7292.186348522175</v>
+      </c>
+      <c r="H44" t="n">
+        <v>5961.786807375215</v>
+      </c>
+      <c r="I44" t="n">
+        <v>10351.08101510932</v>
+      </c>
+      <c r="J44" t="n">
+        <v>9662.839540110737</v>
+      </c>
+      <c r="K44" t="n">
         <v>5938.440200242811</v>
       </c>
-      <c r="B44" t="n">
+      <c r="L44" t="n">
         <v>7995.22065654573</v>
       </c>
-      <c r="C44" t="n">
+      <c r="M44" t="n">
         <v>5752.70945431473</v>
       </c>
-      <c r="D44" t="n">
+      <c r="N44" t="n">
         <v>9273.167824969578</v>
       </c>
-      <c r="E44" t="n">
+      <c r="O44" t="n">
         <v>13468.61370055441</v>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="P44" t="inlineStr">
         <is>
           <t>43º</t>
         </is>
@@ -1413,21 +2753,51 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
+        <v>70661.16958912501</v>
+      </c>
+      <c r="B45" t="n">
+        <v>6447.152664563586</v>
+      </c>
+      <c r="C45" t="n">
+        <v>10945.29743018011</v>
+      </c>
+      <c r="D45" t="n">
+        <v>52692.02202530653</v>
+      </c>
+      <c r="E45" t="n">
+        <v>9996.16926214556</v>
+      </c>
+      <c r="F45" t="n">
+        <v>6514.497647247478</v>
+      </c>
+      <c r="G45" t="n">
+        <v>9375.458367242178</v>
+      </c>
+      <c r="H45" t="n">
+        <v>7284.294057850852</v>
+      </c>
+      <c r="I45" t="n">
+        <v>21955.4699688472</v>
+      </c>
+      <c r="J45" t="n">
+        <v>6831.826669564553</v>
+      </c>
+      <c r="K45" t="n">
         <v>7109.712203054681</v>
       </c>
-      <c r="B45" t="n">
+      <c r="L45" t="n">
         <v>7107.718031810075</v>
       </c>
-      <c r="C45" t="n">
+      <c r="M45" t="n">
         <v>6490.578361487973</v>
       </c>
-      <c r="D45" t="n">
+      <c r="N45" t="n">
         <v>30844.90260950118</v>
       </c>
-      <c r="E45" t="n">
+      <c r="O45" t="n">
         <v>29897.4249533029</v>
       </c>
-      <c r="F45" t="inlineStr">
+      <c r="P45" t="inlineStr">
         <is>
           <t>44º</t>
         </is>
@@ -1435,21 +2805,51 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
+        <v>37178.68723438164</v>
+      </c>
+      <c r="B46" t="n">
+        <v>6382.438820461313</v>
+      </c>
+      <c r="C46" t="n">
+        <v>7574.367677150399</v>
+      </c>
+      <c r="D46" t="n">
+        <v>12098.51162025915</v>
+      </c>
+      <c r="E46" t="n">
+        <v>6741.666722580495</v>
+      </c>
+      <c r="F46" t="n">
+        <v>6334.371632055557</v>
+      </c>
+      <c r="G46" t="n">
+        <v>7439.992977041486</v>
+      </c>
+      <c r="H46" t="n">
+        <v>6098.336568133153</v>
+      </c>
+      <c r="I46" t="n">
+        <v>12799.49303542609</v>
+      </c>
+      <c r="J46" t="n">
+        <v>7234.096068204272</v>
+      </c>
+      <c r="K46" t="n">
         <v>6240.870806815336</v>
       </c>
-      <c r="B46" t="n">
+      <c r="L46" t="n">
         <v>9676.689950343665</v>
       </c>
-      <c r="C46" t="n">
+      <c r="M46" t="n">
         <v>12054.9531064106</v>
       </c>
-      <c r="D46" t="n">
+      <c r="N46" t="n">
         <v>13134.42087425953</v>
       </c>
-      <c r="E46" t="n">
+      <c r="O46" t="n">
         <v>27707.01309284839</v>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="P46" t="inlineStr">
         <is>
           <t>45º</t>
         </is>
@@ -1457,21 +2857,51 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
+        <v>24933.38856977878</v>
+      </c>
+      <c r="B47" t="n">
+        <v>5928.799473721262</v>
+      </c>
+      <c r="C47" t="n">
+        <v>32672.40699014895</v>
+      </c>
+      <c r="D47" t="n">
+        <v>14099.130891567</v>
+      </c>
+      <c r="E47" t="n">
+        <v>5861.28436387614</v>
+      </c>
+      <c r="F47" t="n">
+        <v>21346.11490923024</v>
+      </c>
+      <c r="G47" t="n">
+        <v>8937.291583803717</v>
+      </c>
+      <c r="H47" t="n">
+        <v>5561.367057529263</v>
+      </c>
+      <c r="I47" t="n">
+        <v>6072.917269321749</v>
+      </c>
+      <c r="J47" t="n">
+        <v>33333.05053645021</v>
+      </c>
+      <c r="K47" t="n">
         <v>5511.202952841565</v>
       </c>
-      <c r="B47" t="n">
+      <c r="L47" t="n">
         <v>33211.06589165011</v>
       </c>
-      <c r="C47" t="n">
+      <c r="M47" t="n">
         <v>9484.93085372285</v>
       </c>
-      <c r="D47" t="n">
+      <c r="N47" t="n">
         <v>17566.50619275056</v>
       </c>
-      <c r="E47" t="n">
+      <c r="O47" t="n">
         <v>8392.054353627273</v>
       </c>
-      <c r="F47" t="inlineStr">
+      <c r="P47" t="inlineStr">
         <is>
           <t>46º</t>
         </is>
@@ -1479,21 +2909,51 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
+        <v>5672.270066122799</v>
+      </c>
+      <c r="B48" t="n">
+        <v>9097.766572709177</v>
+      </c>
+      <c r="C48" t="n">
+        <v>56012.19977162862</v>
+      </c>
+      <c r="D48" t="n">
+        <v>41580.16544769507</v>
+      </c>
+      <c r="E48" t="n">
+        <v>14283.55250096229</v>
+      </c>
+      <c r="F48" t="n">
+        <v>31728.18929302273</v>
+      </c>
+      <c r="G48" t="n">
+        <v>6012.728318161241</v>
+      </c>
+      <c r="H48" t="n">
+        <v>4930.356795894055</v>
+      </c>
+      <c r="I48" t="n">
+        <v>5666.021841884708</v>
+      </c>
+      <c r="J48" t="n">
+        <v>49414.52487446283</v>
+      </c>
+      <c r="K48" t="n">
         <v>5124.050996651952</v>
       </c>
-      <c r="B48" t="n">
+      <c r="L48" t="n">
         <v>16712.4859787892</v>
       </c>
-      <c r="C48" t="n">
+      <c r="M48" t="n">
         <v>5561.15559249006</v>
       </c>
-      <c r="D48" t="n">
+      <c r="N48" t="n">
         <v>80767.45710533763</v>
       </c>
-      <c r="E48" t="n">
+      <c r="O48" t="n">
         <v>9129.527045047758</v>
       </c>
-      <c r="F48" t="inlineStr">
+      <c r="P48" t="inlineStr">
         <is>
           <t>47º</t>
         </is>
@@ -1501,21 +2961,51 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
+        <v>8421.17331992574</v>
+      </c>
+      <c r="B49" t="n">
+        <v>18876.62436936601</v>
+      </c>
+      <c r="C49" t="n">
+        <v>70227.62469654922</v>
+      </c>
+      <c r="D49" t="n">
+        <v>6439.55627017255</v>
+      </c>
+      <c r="E49" t="n">
+        <v>99125.99464167807</v>
+      </c>
+      <c r="F49" t="n">
+        <v>14494.0372769122</v>
+      </c>
+      <c r="G49" t="n">
+        <v>42908.63427243324</v>
+      </c>
+      <c r="H49" t="n">
+        <v>21523.19272476787</v>
+      </c>
+      <c r="I49" t="n">
+        <v>28259.22569706906</v>
+      </c>
+      <c r="J49" t="n">
+        <v>39254.23975389144</v>
+      </c>
+      <c r="K49" t="n">
         <v>54669.1408901121</v>
       </c>
-      <c r="B49" t="n">
+      <c r="L49" t="n">
         <v>28671.42263410277</v>
       </c>
-      <c r="C49" t="n">
+      <c r="M49" t="n">
         <v>5868.333167052036</v>
       </c>
-      <c r="D49" t="n">
+      <c r="N49" t="n">
         <v>8809.770703293763</v>
       </c>
-      <c r="E49" t="n">
+      <c r="O49" t="n">
         <v>46944.73664763492</v>
       </c>
-      <c r="F49" t="inlineStr">
+      <c r="P49" t="inlineStr">
         <is>
           <t>48º</t>
         </is>
@@ -1523,21 +3013,51 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
+        <v>76273.41400614539</v>
+      </c>
+      <c r="B50" t="n">
+        <v>130045.5867317013</v>
+      </c>
+      <c r="C50" t="n">
+        <v>9587.127803987376</v>
+      </c>
+      <c r="D50" t="n">
+        <v>23093.50629737426</v>
+      </c>
+      <c r="E50" t="n">
+        <v>46560.00706109909</v>
+      </c>
+      <c r="F50" t="n">
+        <v>16680.25525106915</v>
+      </c>
+      <c r="G50" t="n">
+        <v>8744.372281233927</v>
+      </c>
+      <c r="H50" t="n">
+        <v>14626.27254978069</v>
+      </c>
+      <c r="I50" t="n">
+        <v>24514.08208072562</v>
+      </c>
+      <c r="J50" t="n">
+        <v>14115.1499248584</v>
+      </c>
+      <c r="K50" t="n">
         <v>67251.56909290013</v>
       </c>
-      <c r="B50" t="n">
+      <c r="L50" t="n">
         <v>27354.46760841727</v>
       </c>
-      <c r="C50" t="n">
+      <c r="M50" t="n">
         <v>15557.70649460623</v>
       </c>
-      <c r="D50" t="n">
+      <c r="N50" t="n">
         <v>14062.09529870913</v>
       </c>
-      <c r="E50" t="n">
+      <c r="O50" t="n">
         <v>20449.91481011147</v>
       </c>
-      <c r="F50" t="inlineStr">
+      <c r="P50" t="inlineStr">
         <is>
           <t>49º</t>
         </is>
@@ -1545,21 +3065,51 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
+        <v>18727.61471900989</v>
+      </c>
+      <c r="B51" t="n">
+        <v>31384.67736423718</v>
+      </c>
+      <c r="C51" t="n">
+        <v>60257.27014628023</v>
+      </c>
+      <c r="D51" t="n">
+        <v>96526.69611806681</v>
+      </c>
+      <c r="E51" t="n">
+        <v>10011.37907449358</v>
+      </c>
+      <c r="F51" t="n">
+        <v>24268.06186508805</v>
+      </c>
+      <c r="G51" t="n">
+        <v>44812.41349536019</v>
+      </c>
+      <c r="H51" t="n">
+        <v>27406.92080192845</v>
+      </c>
+      <c r="I51" t="n">
+        <v>21954.69238184664</v>
+      </c>
+      <c r="J51" t="n">
+        <v>11575.73641811773</v>
+      </c>
+      <c r="K51" t="n">
         <v>6365.77879867788</v>
       </c>
-      <c r="B51" t="n">
+      <c r="L51" t="n">
         <v>36631.59455774529</v>
       </c>
-      <c r="C51" t="n">
+      <c r="M51" t="n">
         <v>18531.79274847414</v>
       </c>
-      <c r="D51" t="n">
+      <c r="N51" t="n">
         <v>95751.70509251804</v>
       </c>
-      <c r="E51" t="n">
+      <c r="O51" t="n">
         <v>42907.17247465028</v>
       </c>
-      <c r="F51" t="inlineStr">
+      <c r="P51" t="inlineStr">
         <is>
           <t>50º</t>
         </is>
@@ -1567,21 +3117,51 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
+        <v>88647.65877798475</v>
+      </c>
+      <c r="B52" t="n">
+        <v>63500.89243723355</v>
+      </c>
+      <c r="C52" t="n">
+        <v>43478.7564575784</v>
+      </c>
+      <c r="D52" t="n">
+        <v>7343.835464580618</v>
+      </c>
+      <c r="E52" t="n">
+        <v>6309.283048621806</v>
+      </c>
+      <c r="F52" t="n">
+        <v>29619.03418045091</v>
+      </c>
+      <c r="G52" t="n">
+        <v>15625.06353690811</v>
+      </c>
+      <c r="H52" t="n">
+        <v>27723.09482790398</v>
+      </c>
+      <c r="I52" t="n">
+        <v>30161.58936146054</v>
+      </c>
+      <c r="J52" t="n">
+        <v>17576.82208588358</v>
+      </c>
+      <c r="K52" t="n">
         <v>34482.10052975859</v>
       </c>
-      <c r="B52" t="n">
+      <c r="L52" t="n">
         <v>60486.16977535694</v>
       </c>
-      <c r="C52" t="n">
+      <c r="M52" t="n">
         <v>17544.3230947962</v>
       </c>
-      <c r="D52" t="n">
+      <c r="N52" t="n">
         <v>68415.92054938711</v>
       </c>
-      <c r="E52" t="n">
+      <c r="O52" t="n">
         <v>51386.19000660953</v>
       </c>
-      <c r="F52" t="inlineStr">
+      <c r="P52" t="inlineStr">
         <is>
           <t>51º</t>
         </is>
@@ -1589,21 +3169,51 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
+        <v>58703.37793235595</v>
+      </c>
+      <c r="B53" t="n">
+        <v>56192.07614500756</v>
+      </c>
+      <c r="C53" t="n">
+        <v>20738.49265219324</v>
+      </c>
+      <c r="D53" t="n">
+        <v>57446.49926566147</v>
+      </c>
+      <c r="E53" t="n">
+        <v>23899.14353126825</v>
+      </c>
+      <c r="F53" t="n">
+        <v>5976.203107599886</v>
+      </c>
+      <c r="G53" t="n">
+        <v>26284.76704967442</v>
+      </c>
+      <c r="H53" t="n">
+        <v>63074.95821662419</v>
+      </c>
+      <c r="I53" t="n">
+        <v>12762.17680278012</v>
+      </c>
+      <c r="J53" t="n">
+        <v>55566.75233282577</v>
+      </c>
+      <c r="K53" t="n">
         <v>16944.94792045028</v>
       </c>
-      <c r="B53" t="n">
+      <c r="L53" t="n">
         <v>40628.41183137333</v>
       </c>
-      <c r="C53" t="n">
+      <c r="M53" t="n">
         <v>20586.26380807838</v>
       </c>
-      <c r="D53" t="n">
+      <c r="N53" t="n">
         <v>14449.56290546306</v>
       </c>
-      <c r="E53" t="n">
+      <c r="O53" t="n">
         <v>44692.81962394897</v>
       </c>
-      <c r="F53" t="inlineStr">
+      <c r="P53" t="inlineStr">
         <is>
           <t>52º</t>
         </is>
@@ -1611,21 +3221,51 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
+        <v>63453.94418308773</v>
+      </c>
+      <c r="B54" t="n">
+        <v>60964.35444645696</v>
+      </c>
+      <c r="C54" t="n">
+        <v>16038.51201323434</v>
+      </c>
+      <c r="D54" t="n">
+        <v>65700.5331406761</v>
+      </c>
+      <c r="E54" t="n">
+        <v>33446.16180362094</v>
+      </c>
+      <c r="F54" t="n">
+        <v>14278.0525828628</v>
+      </c>
+      <c r="G54" t="n">
+        <v>79759.2090198142</v>
+      </c>
+      <c r="H54" t="n">
+        <v>45020.76308655358</v>
+      </c>
+      <c r="I54" t="n">
+        <v>28204.34381368138</v>
+      </c>
+      <c r="J54" t="n">
+        <v>79949.97200811427</v>
+      </c>
+      <c r="K54" t="n">
         <v>12396.88754673282</v>
       </c>
-      <c r="B54" t="n">
+      <c r="L54" t="n">
         <v>41581.78839633603</v>
       </c>
-      <c r="C54" t="n">
+      <c r="M54" t="n">
         <v>65273.62896004848</v>
       </c>
-      <c r="D54" t="n">
+      <c r="N54" t="n">
         <v>11972.75249482043</v>
       </c>
-      <c r="E54" t="n">
+      <c r="O54" t="n">
         <v>38746.9641356477</v>
       </c>
-      <c r="F54" t="inlineStr">
+      <c r="P54" t="inlineStr">
         <is>
           <t>53º</t>
         </is>
@@ -1633,21 +3273,51 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
+        <v>15917.08224273218</v>
+      </c>
+      <c r="B55" t="n">
+        <v>76496.85408683112</v>
+      </c>
+      <c r="C55" t="n">
+        <v>71197.89594849409</v>
+      </c>
+      <c r="D55" t="n">
+        <v>68435.00512704661</v>
+      </c>
+      <c r="E55" t="n">
+        <v>57144.4037383341</v>
+      </c>
+      <c r="F55" t="n">
+        <v>59165.34726855515</v>
+      </c>
+      <c r="G55" t="n">
+        <v>77257.54609850724</v>
+      </c>
+      <c r="H55" t="n">
+        <v>13551.41728508192</v>
+      </c>
+      <c r="I55" t="n">
+        <v>37696.8814347828</v>
+      </c>
+      <c r="J55" t="n">
+        <v>40273.82436368051</v>
+      </c>
+      <c r="K55" t="n">
         <v>18476.6768110308</v>
       </c>
-      <c r="B55" t="n">
+      <c r="L55" t="n">
         <v>37475.98969230746</v>
       </c>
-      <c r="C55" t="n">
+      <c r="M55" t="n">
         <v>77315.59558859802</v>
       </c>
-      <c r="D55" t="n">
+      <c r="N55" t="n">
         <v>23368.60965297178</v>
       </c>
-      <c r="E55" t="n">
+      <c r="O55" t="n">
         <v>15863.54590524318</v>
       </c>
-      <c r="F55" t="inlineStr">
+      <c r="P55" t="inlineStr">
         <is>
           <t>54º</t>
         </is>
@@ -1655,21 +3325,51 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
+        <v>41118.72268427027</v>
+      </c>
+      <c r="B56" t="n">
+        <v>31367.59829423029</v>
+      </c>
+      <c r="C56" t="n">
+        <v>17567.86524794148</v>
+      </c>
+      <c r="D56" t="n">
+        <v>39838.27669512614</v>
+      </c>
+      <c r="E56" t="n">
+        <v>53199.29921694272</v>
+      </c>
+      <c r="F56" t="n">
+        <v>36074.55265650841</v>
+      </c>
+      <c r="G56" t="n">
+        <v>85631.41460065276</v>
+      </c>
+      <c r="H56" t="n">
+        <v>17904.42516709753</v>
+      </c>
+      <c r="I56" t="n">
+        <v>96964.57086554407</v>
+      </c>
+      <c r="J56" t="n">
+        <v>30216.22211714352</v>
+      </c>
+      <c r="K56" t="n">
         <v>91882.93851458238</v>
       </c>
-      <c r="B56" t="n">
+      <c r="L56" t="n">
         <v>50064.18270688902</v>
       </c>
-      <c r="C56" t="n">
+      <c r="M56" t="n">
         <v>116485.3516897426</v>
       </c>
-      <c r="D56" t="n">
+      <c r="N56" t="n">
         <v>116839.3243226819</v>
       </c>
-      <c r="E56" t="n">
+      <c r="O56" t="n">
         <v>95732.11622735953</v>
       </c>
-      <c r="F56" t="inlineStr">
+      <c r="P56" t="inlineStr">
         <is>
           <t>55º</t>
         </is>
@@ -1677,21 +3377,51 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
+        <v>66240.97578386044</v>
+      </c>
+      <c r="B57" t="n">
+        <v>34513.76286415215</v>
+      </c>
+      <c r="C57" t="n">
+        <v>81523.47807620374</v>
+      </c>
+      <c r="D57" t="n">
+        <v>103584.2862613678</v>
+      </c>
+      <c r="E57" t="n">
+        <v>31820.75520499734</v>
+      </c>
+      <c r="F57" t="n">
+        <v>73470.08517558535</v>
+      </c>
+      <c r="G57" t="n">
+        <v>96729.02625830041</v>
+      </c>
+      <c r="H57" t="n">
+        <v>94698.8006853066</v>
+      </c>
+      <c r="I57" t="n">
+        <v>19576.50541982535</v>
+      </c>
+      <c r="J57" t="n">
+        <v>34256.87175018321</v>
+      </c>
+      <c r="K57" t="n">
         <v>43601.77344259326</v>
       </c>
-      <c r="B57" t="n">
+      <c r="L57" t="n">
         <v>68786.24854553639</v>
       </c>
-      <c r="C57" t="n">
+      <c r="M57" t="n">
         <v>80559.90952299166</v>
       </c>
-      <c r="D57" t="n">
+      <c r="N57" t="n">
         <v>62567.21029275256</v>
       </c>
-      <c r="E57" t="n">
+      <c r="O57" t="n">
         <v>80212.50486300047</v>
       </c>
-      <c r="F57" t="inlineStr">
+      <c r="P57" t="inlineStr">
         <is>
           <t>56º</t>
         </is>
@@ -1699,21 +3429,51 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
+        <v>50995.29406398888</v>
+      </c>
+      <c r="B58" t="n">
+        <v>101076.2055797951</v>
+      </c>
+      <c r="C58" t="n">
+        <v>56967.3304101495</v>
+      </c>
+      <c r="D58" t="n">
+        <v>47663.02047871743</v>
+      </c>
+      <c r="E58" t="n">
+        <v>95154.22227631748</v>
+      </c>
+      <c r="F58" t="n">
+        <v>101546.0020051319</v>
+      </c>
+      <c r="G58" t="n">
+        <v>90739.76164801352</v>
+      </c>
+      <c r="H58" t="n">
+        <v>112868.2105450687</v>
+      </c>
+      <c r="I58" t="n">
+        <v>48115.43192263768</v>
+      </c>
+      <c r="J58" t="n">
+        <v>74298.92258311063</v>
+      </c>
+      <c r="K58" t="n">
         <v>34728.162439754</v>
       </c>
-      <c r="B58" t="n">
+      <c r="L58" t="n">
         <v>70198.32227344134</v>
       </c>
-      <c r="C58" t="n">
+      <c r="M58" t="n">
         <v>71397.5588944753</v>
       </c>
-      <c r="D58" t="n">
+      <c r="N58" t="n">
         <v>124464.489248646</v>
       </c>
-      <c r="E58" t="n">
+      <c r="O58" t="n">
         <v>91771.86634309053</v>
       </c>
-      <c r="F58" t="inlineStr">
+      <c r="P58" t="inlineStr">
         <is>
           <t>57º</t>
         </is>
@@ -1721,21 +3481,51 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
+        <v>64161.32596591873</v>
+      </c>
+      <c r="B59" t="n">
+        <v>140237.7239530528</v>
+      </c>
+      <c r="C59" t="n">
+        <v>60981.44078156523</v>
+      </c>
+      <c r="D59" t="n">
+        <v>21140.43866644022</v>
+      </c>
+      <c r="E59" t="n">
+        <v>84135.76777500829</v>
+      </c>
+      <c r="F59" t="n">
+        <v>144016.4441775902</v>
+      </c>
+      <c r="G59" t="n">
+        <v>78020.00976086968</v>
+      </c>
+      <c r="H59" t="n">
+        <v>120459.084278735</v>
+      </c>
+      <c r="I59" t="n">
+        <v>66086.48149144792</v>
+      </c>
+      <c r="J59" t="n">
+        <v>84401.95485675285</v>
+      </c>
+      <c r="K59" t="n">
         <v>64860.30762262716</v>
       </c>
-      <c r="B59" t="n">
+      <c r="L59" t="n">
         <v>127095.3240244735</v>
       </c>
-      <c r="C59" t="n">
+      <c r="M59" t="n">
         <v>62237.62112878913</v>
       </c>
-      <c r="D59" t="n">
+      <c r="N59" t="n">
         <v>117504.4122177349</v>
       </c>
-      <c r="E59" t="n">
+      <c r="O59" t="n">
         <v>58668.5128910672</v>
       </c>
-      <c r="F59" t="inlineStr">
+      <c r="P59" t="inlineStr">
         <is>
           <t>58º</t>
         </is>
@@ -1743,21 +3533,51 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
+        <v>118018.3752258376</v>
+      </c>
+      <c r="B60" t="n">
+        <v>109645.0159778745</v>
+      </c>
+      <c r="C60" t="n">
+        <v>64911.42204515232</v>
+      </c>
+      <c r="D60" t="n">
+        <v>77240.01298305107</v>
+      </c>
+      <c r="E60" t="n">
+        <v>86911.56890542264</v>
+      </c>
+      <c r="F60" t="n">
+        <v>39427.88691526861</v>
+      </c>
+      <c r="G60" t="n">
+        <v>85744.40901469064</v>
+      </c>
+      <c r="H60" t="n">
+        <v>77235.56487943609</v>
+      </c>
+      <c r="I60" t="n">
+        <v>50410.90586813946</v>
+      </c>
+      <c r="J60" t="n">
+        <v>75458.25742317272</v>
+      </c>
+      <c r="K60" t="n">
         <v>108523.7861447127</v>
       </c>
-      <c r="B60" t="n">
+      <c r="L60" t="n">
         <v>30974.84711787889</v>
       </c>
-      <c r="C60" t="n">
+      <c r="M60" t="n">
         <v>38623.2799161911</v>
       </c>
-      <c r="D60" t="n">
+      <c r="N60" t="n">
         <v>54878.33303743624</v>
       </c>
-      <c r="E60" t="n">
+      <c r="O60" t="n">
         <v>133084.7158856936</v>
       </c>
-      <c r="F60" t="inlineStr">
+      <c r="P60" t="inlineStr">
         <is>
           <t>59º</t>
         </is>
@@ -1765,21 +3585,51 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
+        <v>192345.3330397961</v>
+      </c>
+      <c r="B61" t="n">
+        <v>113347.4040918276</v>
+      </c>
+      <c r="C61" t="n">
+        <v>124802.5323644601</v>
+      </c>
+      <c r="D61" t="n">
+        <v>137779.6014475278</v>
+      </c>
+      <c r="E61" t="n">
+        <v>88917.41051696331</v>
+      </c>
+      <c r="F61" t="n">
+        <v>89229.72452664116</v>
+      </c>
+      <c r="G61" t="n">
+        <v>94078.81313464967</v>
+      </c>
+      <c r="H61" t="n">
+        <v>74217.74028946375</v>
+      </c>
+      <c r="I61" t="n">
+        <v>80192.82911315984</v>
+      </c>
+      <c r="J61" t="n">
+        <v>102134.5996045207</v>
+      </c>
+      <c r="K61" t="n">
         <v>103998.9556717592</v>
       </c>
-      <c r="B61" t="n">
+      <c r="L61" t="n">
         <v>67461.66697073917</v>
       </c>
-      <c r="C61" t="n">
+      <c r="M61" t="n">
         <v>60101.66248672704</v>
       </c>
-      <c r="D61" t="n">
+      <c r="N61" t="n">
         <v>142244.5946205738</v>
       </c>
-      <c r="E61" t="n">
+      <c r="O61" t="n">
         <v>87045.96627840531</v>
       </c>
-      <c r="F61" t="inlineStr">
+      <c r="P61" t="inlineStr">
         <is>
           <t>60º</t>
         </is>
@@ -1787,21 +3637,51 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
+        <v>174289.0893681096</v>
+      </c>
+      <c r="B62" t="n">
+        <v>171111.7776753146</v>
+      </c>
+      <c r="C62" t="n">
+        <v>113860.3085699157</v>
+      </c>
+      <c r="D62" t="n">
+        <v>23726.03549938319</v>
+      </c>
+      <c r="E62" t="n">
+        <v>85635.15814802508</v>
+      </c>
+      <c r="F62" t="n">
+        <v>42248.93929659431</v>
+      </c>
+      <c r="G62" t="n">
+        <v>173726.4064839008</v>
+      </c>
+      <c r="H62" t="n">
+        <v>178080.0314686793</v>
+      </c>
+      <c r="I62" t="n">
+        <v>46845.74814327552</v>
+      </c>
+      <c r="J62" t="n">
+        <v>128986.6483158037</v>
+      </c>
+      <c r="K62" t="n">
         <v>76661.49234977036</v>
       </c>
-      <c r="B62" t="n">
+      <c r="L62" t="n">
         <v>83668.51396812082</v>
       </c>
-      <c r="C62" t="n">
+      <c r="M62" t="n">
         <v>72202.96159374197</v>
       </c>
-      <c r="D62" t="n">
+      <c r="N62" t="n">
         <v>136798.8767660666</v>
       </c>
-      <c r="E62" t="n">
+      <c r="O62" t="n">
         <v>96756.82982602205</v>
       </c>
-      <c r="F62" t="inlineStr">
+      <c r="P62" t="inlineStr">
         <is>
           <t>61º</t>
         </is>
@@ -1809,21 +3689,51 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
+        <v>90176.92313291891</v>
+      </c>
+      <c r="B63" t="n">
+        <v>48690.13742311864</v>
+      </c>
+      <c r="C63" t="n">
+        <v>74845.10294293496</v>
+      </c>
+      <c r="D63" t="n">
+        <v>130839.6604762059</v>
+      </c>
+      <c r="E63" t="n">
+        <v>108807.3100566789</v>
+      </c>
+      <c r="F63" t="n">
+        <v>107248.7027535083</v>
+      </c>
+      <c r="G63" t="n">
+        <v>83113.84495038052</v>
+      </c>
+      <c r="H63" t="n">
+        <v>64183.66587688791</v>
+      </c>
+      <c r="I63" t="n">
+        <v>54640.90991019823</v>
+      </c>
+      <c r="J63" t="n">
+        <v>198924.9324849673</v>
+      </c>
+      <c r="K63" t="n">
         <v>55695.21592201155</v>
       </c>
-      <c r="B63" t="n">
+      <c r="L63" t="n">
         <v>60240.8104734122</v>
       </c>
-      <c r="C63" t="n">
+      <c r="M63" t="n">
         <v>54257.41824889789</v>
       </c>
-      <c r="D63" t="n">
+      <c r="N63" t="n">
         <v>57544.1217162731</v>
       </c>
-      <c r="E63" t="n">
+      <c r="O63" t="n">
         <v>152106.6095990349</v>
       </c>
-      <c r="F63" t="inlineStr">
+      <c r="P63" t="inlineStr">
         <is>
           <t>62º</t>
         </is>
@@ -1831,21 +3741,51 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
+        <v>91124.43128157975</v>
+      </c>
+      <c r="B64" t="n">
+        <v>31692.9921176992</v>
+      </c>
+      <c r="C64" t="n">
+        <v>162830.4153596615</v>
+      </c>
+      <c r="D64" t="n">
+        <v>72425.97302289102</v>
+      </c>
+      <c r="E64" t="n">
+        <v>146880.4320442535</v>
+      </c>
+      <c r="F64" t="n">
+        <v>114696.7282983071</v>
+      </c>
+      <c r="G64" t="n">
+        <v>25734.01111885144</v>
+      </c>
+      <c r="H64" t="n">
+        <v>104628.8533704046</v>
+      </c>
+      <c r="I64" t="n">
+        <v>103747.8973299475</v>
+      </c>
+      <c r="J64" t="n">
+        <v>80467.36841233575</v>
+      </c>
+      <c r="K64" t="n">
         <v>97993.06354520652</v>
       </c>
-      <c r="B64" t="n">
+      <c r="L64" t="n">
         <v>113198.916695621</v>
       </c>
-      <c r="C64" t="n">
+      <c r="M64" t="n">
         <v>148349.559598115</v>
       </c>
-      <c r="D64" t="n">
+      <c r="N64" t="n">
         <v>146044.7980714986</v>
       </c>
-      <c r="E64" t="n">
+      <c r="O64" t="n">
         <v>153310.9237694461</v>
       </c>
-      <c r="F64" t="inlineStr">
+      <c r="P64" t="inlineStr">
         <is>
           <t>63º</t>
         </is>
@@ -1853,21 +3793,51 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
+        <v>23703.81877560104</v>
+      </c>
+      <c r="B65" t="n">
+        <v>95354.10578947254</v>
+      </c>
+      <c r="C65" t="n">
+        <v>36085.07775345879</v>
+      </c>
+      <c r="D65" t="n">
+        <v>108918.4938325284</v>
+      </c>
+      <c r="E65" t="n">
+        <v>105682.4715886285</v>
+      </c>
+      <c r="F65" t="n">
+        <v>61694.32813654318</v>
+      </c>
+      <c r="G65" t="n">
+        <v>72782.36021516832</v>
+      </c>
+      <c r="H65" t="n">
+        <v>81720.27210218774</v>
+      </c>
+      <c r="I65" t="n">
+        <v>167276.7784229651</v>
+      </c>
+      <c r="J65" t="n">
+        <v>59720.58170318975</v>
+      </c>
+      <c r="K65" t="n">
         <v>80253.28189507656</v>
       </c>
-      <c r="B65" t="n">
+      <c r="L65" t="n">
         <v>104269.3931698742</v>
       </c>
-      <c r="C65" t="n">
+      <c r="M65" t="n">
         <v>117152.9756936279</v>
       </c>
-      <c r="D65" t="n">
+      <c r="N65" t="n">
         <v>116440.4613530177</v>
       </c>
-      <c r="E65" t="n">
+      <c r="O65" t="n">
         <v>150092.1485206472</v>
       </c>
-      <c r="F65" t="inlineStr">
+      <c r="P65" t="inlineStr">
         <is>
           <t>64º</t>
         </is>
@@ -1875,21 +3845,51 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
+        <v>99931.48525912716</v>
+      </c>
+      <c r="B66" t="n">
+        <v>141141.7044611315</v>
+      </c>
+      <c r="C66" t="n">
+        <v>66506.76934751995</v>
+      </c>
+      <c r="D66" t="n">
+        <v>51943.99685995811</v>
+      </c>
+      <c r="E66" t="n">
+        <v>94978.67951409207</v>
+      </c>
+      <c r="F66" t="n">
+        <v>119132.6685980779</v>
+      </c>
+      <c r="G66" t="n">
+        <v>81144.65900836261</v>
+      </c>
+      <c r="H66" t="n">
+        <v>85468.15037463506</v>
+      </c>
+      <c r="I66" t="n">
+        <v>91742.58370023611</v>
+      </c>
+      <c r="J66" t="n">
+        <v>81692.61420562222</v>
+      </c>
+      <c r="K66" t="n">
         <v>139287.0136952719</v>
       </c>
-      <c r="B66" t="n">
+      <c r="L66" t="n">
         <v>85231.12899466876</v>
       </c>
-      <c r="C66" t="n">
+      <c r="M66" t="n">
         <v>104800.6516641392</v>
       </c>
-      <c r="D66" t="n">
+      <c r="N66" t="n">
         <v>177594.6720940085</v>
       </c>
-      <c r="E66" t="n">
+      <c r="O66" t="n">
         <v>169047.2898765191</v>
       </c>
-      <c r="F66" t="inlineStr">
+      <c r="P66" t="inlineStr">
         <is>
           <t>65º</t>
         </is>
@@ -1897,21 +3897,51 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
+        <v>107376.2118392682</v>
+      </c>
+      <c r="B67" t="n">
+        <v>130650.366210672</v>
+      </c>
+      <c r="C67" t="n">
+        <v>66318.71824382714</v>
+      </c>
+      <c r="D67" t="n">
+        <v>70287.75059711802</v>
+      </c>
+      <c r="E67" t="n">
+        <v>104854.2281262603</v>
+      </c>
+      <c r="F67" t="n">
+        <v>107568.8785383505</v>
+      </c>
+      <c r="G67" t="n">
+        <v>98816.75989952849</v>
+      </c>
+      <c r="H67" t="n">
+        <v>180079.1477186689</v>
+      </c>
+      <c r="I67" t="n">
+        <v>90378.64916835472</v>
+      </c>
+      <c r="J67" t="n">
+        <v>44322.14860201021</v>
+      </c>
+      <c r="K67" t="n">
         <v>126354.5323095284</v>
       </c>
-      <c r="B67" t="n">
+      <c r="L67" t="n">
         <v>97838.80656752114</v>
       </c>
-      <c r="C67" t="n">
+      <c r="M67" t="n">
         <v>71977.40978137701</v>
       </c>
-      <c r="D67" t="n">
+      <c r="N67" t="n">
         <v>89753.95373577789</v>
       </c>
-      <c r="E67" t="n">
+      <c r="O67" t="n">
         <v>77924.31629363782</v>
       </c>
-      <c r="F67" t="inlineStr">
+      <c r="P67" t="inlineStr">
         <is>
           <t>66º</t>
         </is>
@@ -1919,21 +3949,51 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
+        <v>105297.1449254204</v>
+      </c>
+      <c r="B68" t="n">
+        <v>135791.9001187868</v>
+      </c>
+      <c r="C68" t="n">
+        <v>109131.000889954</v>
+      </c>
+      <c r="D68" t="n">
+        <v>65127.01511201396</v>
+      </c>
+      <c r="E68" t="n">
+        <v>81539.44658382917</v>
+      </c>
+      <c r="F68" t="n">
+        <v>97140.97002164433</v>
+      </c>
+      <c r="G68" t="n">
+        <v>187999.5763551898</v>
+      </c>
+      <c r="H68" t="n">
+        <v>178530.8829152351</v>
+      </c>
+      <c r="I68" t="n">
+        <v>90487.65841113821</v>
+      </c>
+      <c r="J68" t="n">
+        <v>138086.223970735</v>
+      </c>
+      <c r="K68" t="n">
         <v>66904.14544602179</v>
       </c>
-      <c r="B68" t="n">
+      <c r="L68" t="n">
         <v>90337.63847927767</v>
       </c>
-      <c r="C68" t="n">
+      <c r="M68" t="n">
         <v>146927.201437161</v>
       </c>
-      <c r="D68" t="n">
+      <c r="N68" t="n">
         <v>105837.3174547158</v>
       </c>
-      <c r="E68" t="n">
+      <c r="O68" t="n">
         <v>102581.94035195</v>
       </c>
-      <c r="F68" t="inlineStr">
+      <c r="P68" t="inlineStr">
         <is>
           <t>67º</t>
         </is>
@@ -1941,21 +4001,51 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
+        <v>152117.1130006305</v>
+      </c>
+      <c r="B69" t="n">
+        <v>174168.349567496</v>
+      </c>
+      <c r="C69" t="n">
+        <v>137465.2205697677</v>
+      </c>
+      <c r="D69" t="n">
+        <v>52241.7904372757</v>
+      </c>
+      <c r="E69" t="n">
+        <v>105980.9547960131</v>
+      </c>
+      <c r="F69" t="n">
+        <v>106033.1866210078</v>
+      </c>
+      <c r="G69" t="n">
+        <v>133147.3376299839</v>
+      </c>
+      <c r="H69" t="n">
+        <v>69337.84101466389</v>
+      </c>
+      <c r="I69" t="n">
+        <v>82945.52155364175</v>
+      </c>
+      <c r="J69" t="n">
+        <v>143054.4004942652</v>
+      </c>
+      <c r="K69" t="n">
         <v>46617.18478255177</v>
       </c>
-      <c r="B69" t="n">
+      <c r="L69" t="n">
         <v>112451.0876638898</v>
       </c>
-      <c r="C69" t="n">
+      <c r="M69" t="n">
         <v>85343.36875625304</v>
       </c>
-      <c r="D69" t="n">
+      <c r="N69" t="n">
         <v>77388.24612222092</v>
       </c>
-      <c r="E69" t="n">
+      <c r="O69" t="n">
         <v>81223.37999817706</v>
       </c>
-      <c r="F69" t="inlineStr">
+      <c r="P69" t="inlineStr">
         <is>
           <t>68º</t>
         </is>
@@ -1963,21 +4053,51 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
+        <v>113141.3802612717</v>
+      </c>
+      <c r="B70" t="n">
+        <v>99521.50020686121</v>
+      </c>
+      <c r="C70" t="n">
+        <v>152088.6823558657</v>
+      </c>
+      <c r="D70" t="n">
+        <v>90533.92594454525</v>
+      </c>
+      <c r="E70" t="n">
+        <v>38579.89737969935</v>
+      </c>
+      <c r="F70" t="n">
+        <v>172576.1022968143</v>
+      </c>
+      <c r="G70" t="n">
+        <v>149035.8879049395</v>
+      </c>
+      <c r="H70" t="n">
+        <v>106419.7585988886</v>
+      </c>
+      <c r="I70" t="n">
+        <v>144827.999394024</v>
+      </c>
+      <c r="J70" t="n">
+        <v>167894.0926013796</v>
+      </c>
+      <c r="K70" t="n">
         <v>116587.9999463099</v>
       </c>
-      <c r="B70" t="n">
+      <c r="L70" t="n">
         <v>148440.3311980377</v>
       </c>
-      <c r="C70" t="n">
+      <c r="M70" t="n">
         <v>131785.3621681438</v>
       </c>
-      <c r="D70" t="n">
+      <c r="N70" t="n">
         <v>96867.44785637202</v>
       </c>
-      <c r="E70" t="n">
+      <c r="O70" t="n">
         <v>103365.2585134993</v>
       </c>
-      <c r="F70" t="inlineStr">
+      <c r="P70" t="inlineStr">
         <is>
           <t>69º</t>
         </is>
@@ -1985,21 +4105,51 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
+        <v>70930.17793376406</v>
+      </c>
+      <c r="B71" t="n">
+        <v>139169.8041047939</v>
+      </c>
+      <c r="C71" t="n">
+        <v>204464.1611197159</v>
+      </c>
+      <c r="D71" t="n">
+        <v>106357.4783091489</v>
+      </c>
+      <c r="E71" t="n">
+        <v>127121.3044990165</v>
+      </c>
+      <c r="F71" t="n">
+        <v>178267.3736902873</v>
+      </c>
+      <c r="G71" t="n">
+        <v>103299.0495151855</v>
+      </c>
+      <c r="H71" t="n">
+        <v>105649.2524549596</v>
+      </c>
+      <c r="I71" t="n">
+        <v>114002.4220511642</v>
+      </c>
+      <c r="J71" t="n">
+        <v>187427.7848743664</v>
+      </c>
+      <c r="K71" t="n">
         <v>137264.0334954805</v>
       </c>
-      <c r="B71" t="n">
+      <c r="L71" t="n">
         <v>208159.5676603426</v>
       </c>
-      <c r="C71" t="n">
+      <c r="M71" t="n">
         <v>61077.95498127284</v>
       </c>
-      <c r="D71" t="n">
+      <c r="N71" t="n">
         <v>183138.501261524</v>
       </c>
-      <c r="E71" t="n">
+      <c r="O71" t="n">
         <v>94205.54853680932</v>
       </c>
-      <c r="F71" t="inlineStr">
+      <c r="P71" t="inlineStr">
         <is>
           <t>70º</t>
         </is>
@@ -2007,21 +4157,51 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
+        <v>69818.97708111</v>
+      </c>
+      <c r="B72" t="n">
+        <v>174902.8844040518</v>
+      </c>
+      <c r="C72" t="n">
+        <v>163841.0012723211</v>
+      </c>
+      <c r="D72" t="n">
+        <v>76046.87585558146</v>
+      </c>
+      <c r="E72" t="n">
+        <v>157336.8365210813</v>
+      </c>
+      <c r="F72" t="n">
+        <v>180012.1730222138</v>
+      </c>
+      <c r="G72" t="n">
+        <v>123623.3187921898</v>
+      </c>
+      <c r="H72" t="n">
+        <v>48026.28725962542</v>
+      </c>
+      <c r="I72" t="n">
+        <v>161417.6529249082</v>
+      </c>
+      <c r="J72" t="n">
+        <v>117669.9449438245</v>
+      </c>
+      <c r="K72" t="n">
         <v>76367.68097269772</v>
       </c>
-      <c r="B72" t="n">
+      <c r="L72" t="n">
         <v>184392.233173445</v>
       </c>
-      <c r="C72" t="n">
+      <c r="M72" t="n">
         <v>68871.93074279114</v>
       </c>
-      <c r="D72" t="n">
+      <c r="N72" t="n">
         <v>106535.0017669228</v>
       </c>
-      <c r="E72" t="n">
+      <c r="O72" t="n">
         <v>101567.8479929233</v>
       </c>
-      <c r="F72" t="inlineStr">
+      <c r="P72" t="inlineStr">
         <is>
           <t>71º</t>
         </is>
@@ -2029,21 +4209,51 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
+        <v>136219.6239317911</v>
+      </c>
+      <c r="B73" t="n">
+        <v>141981.2591494541</v>
+      </c>
+      <c r="C73" t="n">
+        <v>121617.3875902849</v>
+      </c>
+      <c r="D73" t="n">
+        <v>171889.9163270986</v>
+      </c>
+      <c r="E73" t="n">
+        <v>267416.9487861186</v>
+      </c>
+      <c r="F73" t="n">
+        <v>227840.3789993887</v>
+      </c>
+      <c r="G73" t="n">
+        <v>156299.3311972525</v>
+      </c>
+      <c r="H73" t="n">
+        <v>167684.8675274792</v>
+      </c>
+      <c r="I73" t="n">
+        <v>226926.1777005066</v>
+      </c>
+      <c r="J73" t="n">
+        <v>132430.2533626631</v>
+      </c>
+      <c r="K73" t="n">
         <v>164132.9249802233</v>
       </c>
-      <c r="B73" t="n">
+      <c r="L73" t="n">
         <v>153835.3393825754</v>
       </c>
-      <c r="C73" t="n">
+      <c r="M73" t="n">
         <v>153910.42203797</v>
       </c>
-      <c r="D73" t="n">
+      <c r="N73" t="n">
         <v>66934.86185870257</v>
       </c>
-      <c r="E73" t="n">
+      <c r="O73" t="n">
         <v>91989.77304216282</v>
       </c>
-      <c r="F73" t="inlineStr">
+      <c r="P73" t="inlineStr">
         <is>
           <t>72º</t>
         </is>

</xml_diff>